<commit_message>
latest changes - shows also score data for german
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\Desktop\langapp\v15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\Desktop\langapp\v17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF5A8F1-8E70-4133-964F-29239CD0911A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA28D49E-39CF-4C96-B0EB-BD28B6F651FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{7340545C-2BB6-4E8B-827D-6673ABB13FB9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7340545C-2BB6-4E8B-827D-6673ABB13FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2880" uniqueCount="1016">
   <si>
     <t>question_text</t>
   </si>
@@ -2665,6 +2665,426 @@
   </si>
   <si>
     <t>160. The verb "sentire" in gerund form is:</t>
+  </si>
+  <si>
+    <t>21. German question</t>
+  </si>
+  <si>
+    <t>22. German question</t>
+  </si>
+  <si>
+    <t>23. German question</t>
+  </si>
+  <si>
+    <t>24. German question</t>
+  </si>
+  <si>
+    <t>25. German question</t>
+  </si>
+  <si>
+    <t>26. German question</t>
+  </si>
+  <si>
+    <t>27. German question</t>
+  </si>
+  <si>
+    <t>28. German question</t>
+  </si>
+  <si>
+    <t>29. German question</t>
+  </si>
+  <si>
+    <t>30. German question</t>
+  </si>
+  <si>
+    <t>31. German question</t>
+  </si>
+  <si>
+    <t>32. German question</t>
+  </si>
+  <si>
+    <t>33. German question</t>
+  </si>
+  <si>
+    <t>34. German question</t>
+  </si>
+  <si>
+    <t>35. German question</t>
+  </si>
+  <si>
+    <t>36. German question</t>
+  </si>
+  <si>
+    <t>37. German question</t>
+  </si>
+  <si>
+    <t>38. German question</t>
+  </si>
+  <si>
+    <t>39. German question</t>
+  </si>
+  <si>
+    <t>40. German question</t>
+  </si>
+  <si>
+    <t>41. German question</t>
+  </si>
+  <si>
+    <t>42. German question</t>
+  </si>
+  <si>
+    <t>43. German question</t>
+  </si>
+  <si>
+    <t>44. German question</t>
+  </si>
+  <si>
+    <t>45. German question</t>
+  </si>
+  <si>
+    <t>46. German question</t>
+  </si>
+  <si>
+    <t>47. German question</t>
+  </si>
+  <si>
+    <t>48. German question</t>
+  </si>
+  <si>
+    <t>49. German question</t>
+  </si>
+  <si>
+    <t>50. German question</t>
+  </si>
+  <si>
+    <t>51. German question</t>
+  </si>
+  <si>
+    <t>52. German question</t>
+  </si>
+  <si>
+    <t>53. German question</t>
+  </si>
+  <si>
+    <t>54. German question</t>
+  </si>
+  <si>
+    <t>55. German question</t>
+  </si>
+  <si>
+    <t>56. German question</t>
+  </si>
+  <si>
+    <t>57. German question</t>
+  </si>
+  <si>
+    <t>58. German question</t>
+  </si>
+  <si>
+    <t>59. German question</t>
+  </si>
+  <si>
+    <t>60. German question</t>
+  </si>
+  <si>
+    <t>61. German question</t>
+  </si>
+  <si>
+    <t>62. German question</t>
+  </si>
+  <si>
+    <t>63. German question</t>
+  </si>
+  <si>
+    <t>64. German question</t>
+  </si>
+  <si>
+    <t>65. German question</t>
+  </si>
+  <si>
+    <t>66. German question</t>
+  </si>
+  <si>
+    <t>67. German question</t>
+  </si>
+  <si>
+    <t>68. German question</t>
+  </si>
+  <si>
+    <t>69. German question</t>
+  </si>
+  <si>
+    <t>70. German question</t>
+  </si>
+  <si>
+    <t>71. German question</t>
+  </si>
+  <si>
+    <t>72. German question</t>
+  </si>
+  <si>
+    <t>73. German question</t>
+  </si>
+  <si>
+    <t>74. German question</t>
+  </si>
+  <si>
+    <t>75. German question</t>
+  </si>
+  <si>
+    <t>76. German question</t>
+  </si>
+  <si>
+    <t>77. German question</t>
+  </si>
+  <si>
+    <t>78. German question</t>
+  </si>
+  <si>
+    <t>79. German question</t>
+  </si>
+  <si>
+    <t>80. German question</t>
+  </si>
+  <si>
+    <t>81. German question</t>
+  </si>
+  <si>
+    <t>82. German question</t>
+  </si>
+  <si>
+    <t>83. German question</t>
+  </si>
+  <si>
+    <t>84. German question</t>
+  </si>
+  <si>
+    <t>85. German question</t>
+  </si>
+  <si>
+    <t>86. German question</t>
+  </si>
+  <si>
+    <t>87. German question</t>
+  </si>
+  <si>
+    <t>88. German question</t>
+  </si>
+  <si>
+    <t>89. German question</t>
+  </si>
+  <si>
+    <t>90. German question</t>
+  </si>
+  <si>
+    <t>91. German question</t>
+  </si>
+  <si>
+    <t>92. German question</t>
+  </si>
+  <si>
+    <t>93. German question</t>
+  </si>
+  <si>
+    <t>94. German question</t>
+  </si>
+  <si>
+    <t>95. German question</t>
+  </si>
+  <si>
+    <t>96. German question</t>
+  </si>
+  <si>
+    <t>97. German question</t>
+  </si>
+  <si>
+    <t>98. German question</t>
+  </si>
+  <si>
+    <t>99. German question</t>
+  </si>
+  <si>
+    <t>100. German question</t>
+  </si>
+  <si>
+    <t>101. German question</t>
+  </si>
+  <si>
+    <t>102. German question</t>
+  </si>
+  <si>
+    <t>103. German question</t>
+  </si>
+  <si>
+    <t>104. German question</t>
+  </si>
+  <si>
+    <t>105. German question</t>
+  </si>
+  <si>
+    <t>106. German question</t>
+  </si>
+  <si>
+    <t>107. German question</t>
+  </si>
+  <si>
+    <t>108. German question</t>
+  </si>
+  <si>
+    <t>109. German question</t>
+  </si>
+  <si>
+    <t>110. German question</t>
+  </si>
+  <si>
+    <t>111. German question</t>
+  </si>
+  <si>
+    <t>112. German question</t>
+  </si>
+  <si>
+    <t>113. German question</t>
+  </si>
+  <si>
+    <t>114. German question</t>
+  </si>
+  <si>
+    <t>115. German question</t>
+  </si>
+  <si>
+    <t>116. German question</t>
+  </si>
+  <si>
+    <t>117. German question</t>
+  </si>
+  <si>
+    <t>118. German question</t>
+  </si>
+  <si>
+    <t>119. German question</t>
+  </si>
+  <si>
+    <t>120. German question</t>
+  </si>
+  <si>
+    <t>121. German question</t>
+  </si>
+  <si>
+    <t>122. German question</t>
+  </si>
+  <si>
+    <t>123. German question</t>
+  </si>
+  <si>
+    <t>124. German question</t>
+  </si>
+  <si>
+    <t>125. German question</t>
+  </si>
+  <si>
+    <t>126. German question</t>
+  </si>
+  <si>
+    <t>127. German question</t>
+  </si>
+  <si>
+    <t>128. German question</t>
+  </si>
+  <si>
+    <t>129. German question</t>
+  </si>
+  <si>
+    <t>130. German question</t>
+  </si>
+  <si>
+    <t>131. German question</t>
+  </si>
+  <si>
+    <t>132. German question</t>
+  </si>
+  <si>
+    <t>133. German question</t>
+  </si>
+  <si>
+    <t>134. German question</t>
+  </si>
+  <si>
+    <t>135. German question</t>
+  </si>
+  <si>
+    <t>136. German question</t>
+  </si>
+  <si>
+    <t>137. German question</t>
+  </si>
+  <si>
+    <t>138. German question</t>
+  </si>
+  <si>
+    <t>139. German question</t>
+  </si>
+  <si>
+    <t>140. German question</t>
+  </si>
+  <si>
+    <t>141. German question</t>
+  </si>
+  <si>
+    <t>142. German question</t>
+  </si>
+  <si>
+    <t>143. German question</t>
+  </si>
+  <si>
+    <t>144. German question</t>
+  </si>
+  <si>
+    <t>145. German question</t>
+  </si>
+  <si>
+    <t>146. German question</t>
+  </si>
+  <si>
+    <t>147. German question</t>
+  </si>
+  <si>
+    <t>148. German question</t>
+  </si>
+  <si>
+    <t>149. German question</t>
+  </si>
+  <si>
+    <t>150. German question</t>
+  </si>
+  <si>
+    <t>151. German question</t>
+  </si>
+  <si>
+    <t>152. German question</t>
+  </si>
+  <si>
+    <t>153. German question</t>
+  </si>
+  <si>
+    <t>154. German question</t>
+  </si>
+  <si>
+    <t>155. German question</t>
+  </si>
+  <si>
+    <t>156. German question</t>
+  </si>
+  <si>
+    <t>157. German question</t>
+  </si>
+  <si>
+    <t>158. German question</t>
+  </si>
+  <si>
+    <t>159. German question</t>
+  </si>
+  <si>
+    <t>160. German question</t>
   </si>
 </sst>
 </file>
@@ -3023,10 +3443,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36A3347-166D-4930-B9BE-A2A96E4C6F8D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H242"/>
+  <dimension ref="A1:H382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="J243" sqref="J243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9323,6 +9743,3646 @@
         <v>689</v>
       </c>
       <c r="H242">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>876</v>
+      </c>
+      <c r="B243" t="s">
+        <v>419</v>
+      </c>
+      <c r="C243" t="s">
+        <v>420</v>
+      </c>
+      <c r="D243" t="s">
+        <v>421</v>
+      </c>
+      <c r="E243" t="s">
+        <v>86</v>
+      </c>
+      <c r="F243" t="s">
+        <v>87</v>
+      </c>
+      <c r="G243" t="s">
+        <v>408</v>
+      </c>
+      <c r="H243">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>877</v>
+      </c>
+      <c r="B244" t="s">
+        <v>422</v>
+      </c>
+      <c r="C244" t="s">
+        <v>423</v>
+      </c>
+      <c r="D244" t="s">
+        <v>424</v>
+      </c>
+      <c r="E244" t="s">
+        <v>86</v>
+      </c>
+      <c r="F244" t="s">
+        <v>87</v>
+      </c>
+      <c r="G244" t="s">
+        <v>408</v>
+      </c>
+      <c r="H244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>878</v>
+      </c>
+      <c r="B245" t="s">
+        <v>425</v>
+      </c>
+      <c r="C245" t="s">
+        <v>426</v>
+      </c>
+      <c r="D245" t="s">
+        <v>427</v>
+      </c>
+      <c r="E245" t="s">
+        <v>86</v>
+      </c>
+      <c r="F245" t="s">
+        <v>87</v>
+      </c>
+      <c r="G245" t="s">
+        <v>408</v>
+      </c>
+      <c r="H245">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>879</v>
+      </c>
+      <c r="B246" t="s">
+        <v>428</v>
+      </c>
+      <c r="C246" t="s">
+        <v>429</v>
+      </c>
+      <c r="D246" t="s">
+        <v>430</v>
+      </c>
+      <c r="E246" t="s">
+        <v>86</v>
+      </c>
+      <c r="F246" t="s">
+        <v>87</v>
+      </c>
+      <c r="G246" t="s">
+        <v>408</v>
+      </c>
+      <c r="H246">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>880</v>
+      </c>
+      <c r="B247" t="s">
+        <v>431</v>
+      </c>
+      <c r="C247" t="s">
+        <v>432</v>
+      </c>
+      <c r="D247" t="s">
+        <v>433</v>
+      </c>
+      <c r="E247" t="s">
+        <v>86</v>
+      </c>
+      <c r="F247" t="s">
+        <v>87</v>
+      </c>
+      <c r="G247" t="s">
+        <v>408</v>
+      </c>
+      <c r="H247">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>881</v>
+      </c>
+      <c r="B248" t="s">
+        <v>434</v>
+      </c>
+      <c r="C248" t="s">
+        <v>435</v>
+      </c>
+      <c r="D248" t="s">
+        <v>436</v>
+      </c>
+      <c r="E248" t="s">
+        <v>86</v>
+      </c>
+      <c r="F248" t="s">
+        <v>87</v>
+      </c>
+      <c r="G248" t="s">
+        <v>408</v>
+      </c>
+      <c r="H248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>882</v>
+      </c>
+      <c r="B249" t="s">
+        <v>437</v>
+      </c>
+      <c r="C249" t="s">
+        <v>438</v>
+      </c>
+      <c r="D249" t="s">
+        <v>439</v>
+      </c>
+      <c r="E249" t="s">
+        <v>86</v>
+      </c>
+      <c r="F249" t="s">
+        <v>87</v>
+      </c>
+      <c r="G249" t="s">
+        <v>408</v>
+      </c>
+      <c r="H249">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>883</v>
+      </c>
+      <c r="B250" t="s">
+        <v>440</v>
+      </c>
+      <c r="C250" t="s">
+        <v>441</v>
+      </c>
+      <c r="D250" t="s">
+        <v>442</v>
+      </c>
+      <c r="E250" t="s">
+        <v>86</v>
+      </c>
+      <c r="F250" t="s">
+        <v>87</v>
+      </c>
+      <c r="G250" t="s">
+        <v>408</v>
+      </c>
+      <c r="H250">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>884</v>
+      </c>
+      <c r="B251" t="s">
+        <v>443</v>
+      </c>
+      <c r="C251" t="s">
+        <v>444</v>
+      </c>
+      <c r="D251" t="s">
+        <v>445</v>
+      </c>
+      <c r="E251" t="s">
+        <v>86</v>
+      </c>
+      <c r="F251" t="s">
+        <v>87</v>
+      </c>
+      <c r="G251" t="s">
+        <v>408</v>
+      </c>
+      <c r="H251">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>885</v>
+      </c>
+      <c r="B252" t="s">
+        <v>446</v>
+      </c>
+      <c r="C252" t="s">
+        <v>447</v>
+      </c>
+      <c r="D252" t="s">
+        <v>448</v>
+      </c>
+      <c r="E252" t="s">
+        <v>86</v>
+      </c>
+      <c r="F252" t="s">
+        <v>87</v>
+      </c>
+      <c r="G252" t="s">
+        <v>408</v>
+      </c>
+      <c r="H252">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>886</v>
+      </c>
+      <c r="B253" t="s">
+        <v>449</v>
+      </c>
+      <c r="C253" t="s">
+        <v>450</v>
+      </c>
+      <c r="D253" t="s">
+        <v>451</v>
+      </c>
+      <c r="E253" t="s">
+        <v>86</v>
+      </c>
+      <c r="F253" t="s">
+        <v>87</v>
+      </c>
+      <c r="G253" t="s">
+        <v>408</v>
+      </c>
+      <c r="H253">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>887</v>
+      </c>
+      <c r="B254" t="s">
+        <v>452</v>
+      </c>
+      <c r="C254" t="s">
+        <v>453</v>
+      </c>
+      <c r="D254" t="s">
+        <v>454</v>
+      </c>
+      <c r="E254" t="s">
+        <v>86</v>
+      </c>
+      <c r="F254" t="s">
+        <v>87</v>
+      </c>
+      <c r="G254" t="s">
+        <v>408</v>
+      </c>
+      <c r="H254">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>888</v>
+      </c>
+      <c r="B255" t="s">
+        <v>455</v>
+      </c>
+      <c r="C255" t="s">
+        <v>456</v>
+      </c>
+      <c r="D255" t="s">
+        <v>457</v>
+      </c>
+      <c r="E255" t="s">
+        <v>86</v>
+      </c>
+      <c r="F255" t="s">
+        <v>87</v>
+      </c>
+      <c r="G255" t="s">
+        <v>408</v>
+      </c>
+      <c r="H255">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>889</v>
+      </c>
+      <c r="B256" t="s">
+        <v>458</v>
+      </c>
+      <c r="C256" t="s">
+        <v>459</v>
+      </c>
+      <c r="D256" t="s">
+        <v>460</v>
+      </c>
+      <c r="E256" t="s">
+        <v>86</v>
+      </c>
+      <c r="F256" t="s">
+        <v>87</v>
+      </c>
+      <c r="G256" t="s">
+        <v>408</v>
+      </c>
+      <c r="H256">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>890</v>
+      </c>
+      <c r="B257" t="s">
+        <v>461</v>
+      </c>
+      <c r="C257" t="s">
+        <v>462</v>
+      </c>
+      <c r="D257" t="s">
+        <v>463</v>
+      </c>
+      <c r="E257" t="s">
+        <v>86</v>
+      </c>
+      <c r="F257" t="s">
+        <v>87</v>
+      </c>
+      <c r="G257" t="s">
+        <v>408</v>
+      </c>
+      <c r="H257">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>891</v>
+      </c>
+      <c r="B258" t="s">
+        <v>464</v>
+      </c>
+      <c r="C258" t="s">
+        <v>465</v>
+      </c>
+      <c r="D258" t="s">
+        <v>466</v>
+      </c>
+      <c r="E258" t="s">
+        <v>86</v>
+      </c>
+      <c r="F258" t="s">
+        <v>87</v>
+      </c>
+      <c r="G258" t="s">
+        <v>408</v>
+      </c>
+      <c r="H258">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>892</v>
+      </c>
+      <c r="B259" t="s">
+        <v>467</v>
+      </c>
+      <c r="C259" t="s">
+        <v>468</v>
+      </c>
+      <c r="D259" t="s">
+        <v>469</v>
+      </c>
+      <c r="E259" t="s">
+        <v>86</v>
+      </c>
+      <c r="F259" t="s">
+        <v>87</v>
+      </c>
+      <c r="G259" t="s">
+        <v>408</v>
+      </c>
+      <c r="H259">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>893</v>
+      </c>
+      <c r="B260" t="s">
+        <v>470</v>
+      </c>
+      <c r="C260" t="s">
+        <v>471</v>
+      </c>
+      <c r="D260" t="s">
+        <v>472</v>
+      </c>
+      <c r="E260" t="s">
+        <v>86</v>
+      </c>
+      <c r="F260" t="s">
+        <v>87</v>
+      </c>
+      <c r="G260" t="s">
+        <v>408</v>
+      </c>
+      <c r="H260">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>894</v>
+      </c>
+      <c r="B261" t="s">
+        <v>473</v>
+      </c>
+      <c r="C261" t="s">
+        <v>474</v>
+      </c>
+      <c r="D261" t="s">
+        <v>475</v>
+      </c>
+      <c r="E261" t="s">
+        <v>86</v>
+      </c>
+      <c r="F261" t="s">
+        <v>87</v>
+      </c>
+      <c r="G261" t="s">
+        <v>408</v>
+      </c>
+      <c r="H261">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>895</v>
+      </c>
+      <c r="B262" t="s">
+        <v>476</v>
+      </c>
+      <c r="C262" t="s">
+        <v>477</v>
+      </c>
+      <c r="D262" t="s">
+        <v>478</v>
+      </c>
+      <c r="E262" t="s">
+        <v>86</v>
+      </c>
+      <c r="F262" t="s">
+        <v>87</v>
+      </c>
+      <c r="G262" t="s">
+        <v>408</v>
+      </c>
+      <c r="H262">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>896</v>
+      </c>
+      <c r="B263" t="s">
+        <v>479</v>
+      </c>
+      <c r="C263" t="s">
+        <v>444</v>
+      </c>
+      <c r="D263" t="s">
+        <v>445</v>
+      </c>
+      <c r="E263" t="s">
+        <v>86</v>
+      </c>
+      <c r="F263" t="s">
+        <v>87</v>
+      </c>
+      <c r="G263" t="s">
+        <v>480</v>
+      </c>
+      <c r="H263">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>897</v>
+      </c>
+      <c r="B264" t="s">
+        <v>481</v>
+      </c>
+      <c r="C264" t="s">
+        <v>482</v>
+      </c>
+      <c r="D264" t="s">
+        <v>483</v>
+      </c>
+      <c r="E264" t="s">
+        <v>86</v>
+      </c>
+      <c r="F264" t="s">
+        <v>87</v>
+      </c>
+      <c r="G264" t="s">
+        <v>480</v>
+      </c>
+      <c r="H264">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>898</v>
+      </c>
+      <c r="B265" t="s">
+        <v>484</v>
+      </c>
+      <c r="C265" t="s">
+        <v>485</v>
+      </c>
+      <c r="D265" t="s">
+        <v>486</v>
+      </c>
+      <c r="E265" t="s">
+        <v>86</v>
+      </c>
+      <c r="F265" t="s">
+        <v>87</v>
+      </c>
+      <c r="G265" t="s">
+        <v>480</v>
+      </c>
+      <c r="H265">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>899</v>
+      </c>
+      <c r="B266" t="s">
+        <v>487</v>
+      </c>
+      <c r="C266" t="s">
+        <v>488</v>
+      </c>
+      <c r="D266" t="s">
+        <v>489</v>
+      </c>
+      <c r="E266" t="s">
+        <v>86</v>
+      </c>
+      <c r="F266" t="s">
+        <v>87</v>
+      </c>
+      <c r="G266" t="s">
+        <v>480</v>
+      </c>
+      <c r="H266">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>900</v>
+      </c>
+      <c r="B267" t="s">
+        <v>490</v>
+      </c>
+      <c r="C267" t="s">
+        <v>491</v>
+      </c>
+      <c r="D267" t="s">
+        <v>492</v>
+      </c>
+      <c r="E267" t="s">
+        <v>86</v>
+      </c>
+      <c r="F267" t="s">
+        <v>87</v>
+      </c>
+      <c r="G267" t="s">
+        <v>480</v>
+      </c>
+      <c r="H267">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>901</v>
+      </c>
+      <c r="B268" t="s">
+        <v>493</v>
+      </c>
+      <c r="C268" t="s">
+        <v>494</v>
+      </c>
+      <c r="D268" t="s">
+        <v>495</v>
+      </c>
+      <c r="E268" t="s">
+        <v>86</v>
+      </c>
+      <c r="F268" t="s">
+        <v>87</v>
+      </c>
+      <c r="G268" t="s">
+        <v>480</v>
+      </c>
+      <c r="H268">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>902</v>
+      </c>
+      <c r="B269" t="s">
+        <v>496</v>
+      </c>
+      <c r="C269" t="s">
+        <v>497</v>
+      </c>
+      <c r="D269" t="s">
+        <v>498</v>
+      </c>
+      <c r="E269" t="s">
+        <v>86</v>
+      </c>
+      <c r="F269" t="s">
+        <v>87</v>
+      </c>
+      <c r="G269" t="s">
+        <v>480</v>
+      </c>
+      <c r="H269">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>903</v>
+      </c>
+      <c r="B270" t="s">
+        <v>499</v>
+      </c>
+      <c r="C270" t="s">
+        <v>441</v>
+      </c>
+      <c r="D270" t="s">
+        <v>442</v>
+      </c>
+      <c r="E270" t="s">
+        <v>86</v>
+      </c>
+      <c r="F270" t="s">
+        <v>87</v>
+      </c>
+      <c r="G270" t="s">
+        <v>480</v>
+      </c>
+      <c r="H270">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>904</v>
+      </c>
+      <c r="B271" t="s">
+        <v>500</v>
+      </c>
+      <c r="C271" t="s">
+        <v>501</v>
+      </c>
+      <c r="D271" t="s">
+        <v>502</v>
+      </c>
+      <c r="E271" t="s">
+        <v>86</v>
+      </c>
+      <c r="F271" t="s">
+        <v>87</v>
+      </c>
+      <c r="G271" t="s">
+        <v>480</v>
+      </c>
+      <c r="H271">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>905</v>
+      </c>
+      <c r="B272" t="s">
+        <v>503</v>
+      </c>
+      <c r="C272" t="s">
+        <v>504</v>
+      </c>
+      <c r="D272" t="s">
+        <v>505</v>
+      </c>
+      <c r="E272" t="s">
+        <v>86</v>
+      </c>
+      <c r="F272" t="s">
+        <v>87</v>
+      </c>
+      <c r="G272" t="s">
+        <v>480</v>
+      </c>
+      <c r="H272">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>906</v>
+      </c>
+      <c r="B273" t="s">
+        <v>506</v>
+      </c>
+      <c r="C273" t="s">
+        <v>450</v>
+      </c>
+      <c r="D273" t="s">
+        <v>451</v>
+      </c>
+      <c r="E273" t="s">
+        <v>86</v>
+      </c>
+      <c r="F273" t="s">
+        <v>87</v>
+      </c>
+      <c r="G273" t="s">
+        <v>480</v>
+      </c>
+      <c r="H273">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>907</v>
+      </c>
+      <c r="B274" t="s">
+        <v>507</v>
+      </c>
+      <c r="C274" t="s">
+        <v>508</v>
+      </c>
+      <c r="D274" t="s">
+        <v>509</v>
+      </c>
+      <c r="E274" t="s">
+        <v>86</v>
+      </c>
+      <c r="F274" t="s">
+        <v>87</v>
+      </c>
+      <c r="G274" t="s">
+        <v>480</v>
+      </c>
+      <c r="H274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>908</v>
+      </c>
+      <c r="B275" t="s">
+        <v>510</v>
+      </c>
+      <c r="C275" t="s">
+        <v>511</v>
+      </c>
+      <c r="D275" t="s">
+        <v>512</v>
+      </c>
+      <c r="E275" t="s">
+        <v>86</v>
+      </c>
+      <c r="F275" t="s">
+        <v>87</v>
+      </c>
+      <c r="G275" t="s">
+        <v>480</v>
+      </c>
+      <c r="H275">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>909</v>
+      </c>
+      <c r="B276" t="s">
+        <v>513</v>
+      </c>
+      <c r="C276" t="s">
+        <v>459</v>
+      </c>
+      <c r="D276" t="s">
+        <v>460</v>
+      </c>
+      <c r="E276" t="s">
+        <v>86</v>
+      </c>
+      <c r="F276" t="s">
+        <v>87</v>
+      </c>
+      <c r="G276" t="s">
+        <v>480</v>
+      </c>
+      <c r="H276">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>910</v>
+      </c>
+      <c r="B277" t="s">
+        <v>514</v>
+      </c>
+      <c r="C277" t="s">
+        <v>515</v>
+      </c>
+      <c r="D277" t="s">
+        <v>516</v>
+      </c>
+      <c r="E277" t="s">
+        <v>86</v>
+      </c>
+      <c r="F277" t="s">
+        <v>87</v>
+      </c>
+      <c r="G277" t="s">
+        <v>480</v>
+      </c>
+      <c r="H277">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>911</v>
+      </c>
+      <c r="B278" t="s">
+        <v>517</v>
+      </c>
+      <c r="C278" t="s">
+        <v>518</v>
+      </c>
+      <c r="D278" t="s">
+        <v>519</v>
+      </c>
+      <c r="E278" t="s">
+        <v>86</v>
+      </c>
+      <c r="F278" t="s">
+        <v>87</v>
+      </c>
+      <c r="G278" t="s">
+        <v>480</v>
+      </c>
+      <c r="H278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>912</v>
+      </c>
+      <c r="B279" t="s">
+        <v>520</v>
+      </c>
+      <c r="C279" t="s">
+        <v>491</v>
+      </c>
+      <c r="D279" t="s">
+        <v>492</v>
+      </c>
+      <c r="E279" t="s">
+        <v>86</v>
+      </c>
+      <c r="F279" t="s">
+        <v>87</v>
+      </c>
+      <c r="G279" t="s">
+        <v>480</v>
+      </c>
+      <c r="H279">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>913</v>
+      </c>
+      <c r="B280" t="s">
+        <v>521</v>
+      </c>
+      <c r="C280" t="s">
+        <v>522</v>
+      </c>
+      <c r="D280" t="s">
+        <v>523</v>
+      </c>
+      <c r="E280" t="s">
+        <v>86</v>
+      </c>
+      <c r="F280" t="s">
+        <v>87</v>
+      </c>
+      <c r="G280" t="s">
+        <v>480</v>
+      </c>
+      <c r="H280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>914</v>
+      </c>
+      <c r="B281" t="s">
+        <v>524</v>
+      </c>
+      <c r="C281" t="s">
+        <v>525</v>
+      </c>
+      <c r="D281" t="s">
+        <v>526</v>
+      </c>
+      <c r="E281" t="s">
+        <v>86</v>
+      </c>
+      <c r="F281" t="s">
+        <v>87</v>
+      </c>
+      <c r="G281" t="s">
+        <v>480</v>
+      </c>
+      <c r="H281">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>915</v>
+      </c>
+      <c r="B282" t="s">
+        <v>527</v>
+      </c>
+      <c r="C282" t="s">
+        <v>528</v>
+      </c>
+      <c r="D282" t="s">
+        <v>529</v>
+      </c>
+      <c r="E282" t="s">
+        <v>86</v>
+      </c>
+      <c r="F282" t="s">
+        <v>87</v>
+      </c>
+      <c r="G282" t="s">
+        <v>480</v>
+      </c>
+      <c r="H282">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>916</v>
+      </c>
+      <c r="B283" t="s">
+        <v>530</v>
+      </c>
+      <c r="C283" t="s">
+        <v>420</v>
+      </c>
+      <c r="D283" t="s">
+        <v>531</v>
+      </c>
+      <c r="E283" t="s">
+        <v>86</v>
+      </c>
+      <c r="F283" t="s">
+        <v>87</v>
+      </c>
+      <c r="G283" t="s">
+        <v>532</v>
+      </c>
+      <c r="H283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>917</v>
+      </c>
+      <c r="B284" t="s">
+        <v>533</v>
+      </c>
+      <c r="C284" t="s">
+        <v>423</v>
+      </c>
+      <c r="D284" t="s">
+        <v>534</v>
+      </c>
+      <c r="E284" t="s">
+        <v>86</v>
+      </c>
+      <c r="F284" t="s">
+        <v>87</v>
+      </c>
+      <c r="G284" t="s">
+        <v>532</v>
+      </c>
+      <c r="H284">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>918</v>
+      </c>
+      <c r="B285" t="s">
+        <v>535</v>
+      </c>
+      <c r="C285" t="s">
+        <v>536</v>
+      </c>
+      <c r="D285" t="s">
+        <v>537</v>
+      </c>
+      <c r="E285" t="s">
+        <v>86</v>
+      </c>
+      <c r="F285" t="s">
+        <v>87</v>
+      </c>
+      <c r="G285" t="s">
+        <v>532</v>
+      </c>
+      <c r="H285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>919</v>
+      </c>
+      <c r="B286" t="s">
+        <v>538</v>
+      </c>
+      <c r="C286" t="s">
+        <v>539</v>
+      </c>
+      <c r="D286" t="s">
+        <v>540</v>
+      </c>
+      <c r="E286" t="s">
+        <v>86</v>
+      </c>
+      <c r="F286" t="s">
+        <v>87</v>
+      </c>
+      <c r="G286" t="s">
+        <v>532</v>
+      </c>
+      <c r="H286">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>920</v>
+      </c>
+      <c r="B287" t="s">
+        <v>541</v>
+      </c>
+      <c r="C287" t="s">
+        <v>542</v>
+      </c>
+      <c r="D287" t="s">
+        <v>543</v>
+      </c>
+      <c r="E287" t="s">
+        <v>86</v>
+      </c>
+      <c r="F287" t="s">
+        <v>87</v>
+      </c>
+      <c r="G287" t="s">
+        <v>532</v>
+      </c>
+      <c r="H287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>921</v>
+      </c>
+      <c r="B288" t="s">
+        <v>544</v>
+      </c>
+      <c r="C288" t="s">
+        <v>545</v>
+      </c>
+      <c r="D288" t="s">
+        <v>546</v>
+      </c>
+      <c r="E288" t="s">
+        <v>86</v>
+      </c>
+      <c r="F288" t="s">
+        <v>87</v>
+      </c>
+      <c r="G288" t="s">
+        <v>532</v>
+      </c>
+      <c r="H288">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>922</v>
+      </c>
+      <c r="B289" t="s">
+        <v>547</v>
+      </c>
+      <c r="C289" t="s">
+        <v>548</v>
+      </c>
+      <c r="D289" t="s">
+        <v>549</v>
+      </c>
+      <c r="E289" t="s">
+        <v>86</v>
+      </c>
+      <c r="F289" t="s">
+        <v>87</v>
+      </c>
+      <c r="G289" t="s">
+        <v>532</v>
+      </c>
+      <c r="H289">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>923</v>
+      </c>
+      <c r="B290" t="s">
+        <v>550</v>
+      </c>
+      <c r="C290" t="s">
+        <v>551</v>
+      </c>
+      <c r="D290" t="s">
+        <v>552</v>
+      </c>
+      <c r="E290" t="s">
+        <v>86</v>
+      </c>
+      <c r="F290" t="s">
+        <v>87</v>
+      </c>
+      <c r="G290" t="s">
+        <v>532</v>
+      </c>
+      <c r="H290">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>924</v>
+      </c>
+      <c r="B291" t="s">
+        <v>553</v>
+      </c>
+      <c r="C291" t="s">
+        <v>554</v>
+      </c>
+      <c r="D291" t="s">
+        <v>555</v>
+      </c>
+      <c r="E291" t="s">
+        <v>86</v>
+      </c>
+      <c r="F291" t="s">
+        <v>87</v>
+      </c>
+      <c r="G291" t="s">
+        <v>532</v>
+      </c>
+      <c r="H291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>925</v>
+      </c>
+      <c r="B292" t="s">
+        <v>556</v>
+      </c>
+      <c r="C292" t="s">
+        <v>557</v>
+      </c>
+      <c r="D292" t="s">
+        <v>558</v>
+      </c>
+      <c r="E292" t="s">
+        <v>86</v>
+      </c>
+      <c r="F292" t="s">
+        <v>87</v>
+      </c>
+      <c r="G292" t="s">
+        <v>532</v>
+      </c>
+      <c r="H292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>926</v>
+      </c>
+      <c r="B293" t="s">
+        <v>559</v>
+      </c>
+      <c r="C293" t="s">
+        <v>560</v>
+      </c>
+      <c r="D293" t="s">
+        <v>561</v>
+      </c>
+      <c r="E293" t="s">
+        <v>86</v>
+      </c>
+      <c r="F293" t="s">
+        <v>87</v>
+      </c>
+      <c r="G293" t="s">
+        <v>532</v>
+      </c>
+      <c r="H293">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>927</v>
+      </c>
+      <c r="B294" t="s">
+        <v>562</v>
+      </c>
+      <c r="C294" t="s">
+        <v>563</v>
+      </c>
+      <c r="D294" t="s">
+        <v>564</v>
+      </c>
+      <c r="E294" t="s">
+        <v>86</v>
+      </c>
+      <c r="F294" t="s">
+        <v>87</v>
+      </c>
+      <c r="G294" t="s">
+        <v>532</v>
+      </c>
+      <c r="H294">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>928</v>
+      </c>
+      <c r="B295" t="s">
+        <v>565</v>
+      </c>
+      <c r="C295" t="s">
+        <v>566</v>
+      </c>
+      <c r="D295" t="s">
+        <v>567</v>
+      </c>
+      <c r="E295" t="s">
+        <v>86</v>
+      </c>
+      <c r="F295" t="s">
+        <v>87</v>
+      </c>
+      <c r="G295" t="s">
+        <v>532</v>
+      </c>
+      <c r="H295">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>929</v>
+      </c>
+      <c r="B296" t="s">
+        <v>568</v>
+      </c>
+      <c r="C296" t="s">
+        <v>468</v>
+      </c>
+      <c r="D296" t="s">
+        <v>569</v>
+      </c>
+      <c r="E296" t="s">
+        <v>86</v>
+      </c>
+      <c r="F296" t="s">
+        <v>87</v>
+      </c>
+      <c r="G296" t="s">
+        <v>532</v>
+      </c>
+      <c r="H296">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>930</v>
+      </c>
+      <c r="B297" t="s">
+        <v>570</v>
+      </c>
+      <c r="C297" t="s">
+        <v>571</v>
+      </c>
+      <c r="D297" t="s">
+        <v>572</v>
+      </c>
+      <c r="E297" t="s">
+        <v>86</v>
+      </c>
+      <c r="F297" t="s">
+        <v>87</v>
+      </c>
+      <c r="G297" t="s">
+        <v>532</v>
+      </c>
+      <c r="H297">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>931</v>
+      </c>
+      <c r="B298" t="s">
+        <v>573</v>
+      </c>
+      <c r="C298" t="s">
+        <v>459</v>
+      </c>
+      <c r="D298" t="s">
+        <v>574</v>
+      </c>
+      <c r="E298" t="s">
+        <v>86</v>
+      </c>
+      <c r="F298" t="s">
+        <v>87</v>
+      </c>
+      <c r="G298" t="s">
+        <v>532</v>
+      </c>
+      <c r="H298">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>932</v>
+      </c>
+      <c r="B299" t="s">
+        <v>575</v>
+      </c>
+      <c r="C299" t="s">
+        <v>576</v>
+      </c>
+      <c r="D299" t="s">
+        <v>577</v>
+      </c>
+      <c r="E299" t="s">
+        <v>86</v>
+      </c>
+      <c r="F299" t="s">
+        <v>87</v>
+      </c>
+      <c r="G299" t="s">
+        <v>532</v>
+      </c>
+      <c r="H299">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>933</v>
+      </c>
+      <c r="B300" t="s">
+        <v>578</v>
+      </c>
+      <c r="C300" t="s">
+        <v>579</v>
+      </c>
+      <c r="D300" t="s">
+        <v>580</v>
+      </c>
+      <c r="E300" t="s">
+        <v>86</v>
+      </c>
+      <c r="F300" t="s">
+        <v>87</v>
+      </c>
+      <c r="G300" t="s">
+        <v>532</v>
+      </c>
+      <c r="H300">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>934</v>
+      </c>
+      <c r="B301" t="s">
+        <v>581</v>
+      </c>
+      <c r="C301" t="s">
+        <v>582</v>
+      </c>
+      <c r="D301" t="s">
+        <v>583</v>
+      </c>
+      <c r="E301" t="s">
+        <v>86</v>
+      </c>
+      <c r="F301" t="s">
+        <v>87</v>
+      </c>
+      <c r="G301" t="s">
+        <v>532</v>
+      </c>
+      <c r="H301">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>935</v>
+      </c>
+      <c r="B302" t="s">
+        <v>584</v>
+      </c>
+      <c r="C302" t="s">
+        <v>585</v>
+      </c>
+      <c r="D302" t="s">
+        <v>586</v>
+      </c>
+      <c r="E302" t="s">
+        <v>86</v>
+      </c>
+      <c r="F302" t="s">
+        <v>87</v>
+      </c>
+      <c r="G302" t="s">
+        <v>532</v>
+      </c>
+      <c r="H302">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>936</v>
+      </c>
+      <c r="B303" t="s">
+        <v>587</v>
+      </c>
+      <c r="C303" t="s">
+        <v>420</v>
+      </c>
+      <c r="D303" t="s">
+        <v>421</v>
+      </c>
+      <c r="E303" t="s">
+        <v>86</v>
+      </c>
+      <c r="F303" t="s">
+        <v>87</v>
+      </c>
+      <c r="G303" t="s">
+        <v>588</v>
+      </c>
+      <c r="H303">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>937</v>
+      </c>
+      <c r="B304" t="s">
+        <v>589</v>
+      </c>
+      <c r="C304" t="s">
+        <v>423</v>
+      </c>
+      <c r="D304" t="s">
+        <v>424</v>
+      </c>
+      <c r="E304" t="s">
+        <v>86</v>
+      </c>
+      <c r="F304" t="s">
+        <v>87</v>
+      </c>
+      <c r="G304" t="s">
+        <v>588</v>
+      </c>
+      <c r="H304">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>938</v>
+      </c>
+      <c r="B305" t="s">
+        <v>590</v>
+      </c>
+      <c r="C305" t="s">
+        <v>536</v>
+      </c>
+      <c r="D305" t="s">
+        <v>591</v>
+      </c>
+      <c r="E305" t="s">
+        <v>86</v>
+      </c>
+      <c r="F305" t="s">
+        <v>87</v>
+      </c>
+      <c r="G305" t="s">
+        <v>588</v>
+      </c>
+      <c r="H305">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>939</v>
+      </c>
+      <c r="B306" t="s">
+        <v>592</v>
+      </c>
+      <c r="C306" t="s">
+        <v>539</v>
+      </c>
+      <c r="D306" t="s">
+        <v>593</v>
+      </c>
+      <c r="E306" t="s">
+        <v>86</v>
+      </c>
+      <c r="F306" t="s">
+        <v>87</v>
+      </c>
+      <c r="G306" t="s">
+        <v>588</v>
+      </c>
+      <c r="H306">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>940</v>
+      </c>
+      <c r="B307" t="s">
+        <v>594</v>
+      </c>
+      <c r="C307" t="s">
+        <v>542</v>
+      </c>
+      <c r="D307" t="s">
+        <v>595</v>
+      </c>
+      <c r="E307" t="s">
+        <v>86</v>
+      </c>
+      <c r="F307" t="s">
+        <v>87</v>
+      </c>
+      <c r="G307" t="s">
+        <v>588</v>
+      </c>
+      <c r="H307">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>941</v>
+      </c>
+      <c r="B308" t="s">
+        <v>596</v>
+      </c>
+      <c r="C308" t="s">
+        <v>545</v>
+      </c>
+      <c r="D308" t="s">
+        <v>597</v>
+      </c>
+      <c r="E308" t="s">
+        <v>86</v>
+      </c>
+      <c r="F308" t="s">
+        <v>87</v>
+      </c>
+      <c r="G308" t="s">
+        <v>588</v>
+      </c>
+      <c r="H308">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>942</v>
+      </c>
+      <c r="B309" t="s">
+        <v>598</v>
+      </c>
+      <c r="C309" t="s">
+        <v>548</v>
+      </c>
+      <c r="D309" t="s">
+        <v>599</v>
+      </c>
+      <c r="E309" t="s">
+        <v>86</v>
+      </c>
+      <c r="F309" t="s">
+        <v>87</v>
+      </c>
+      <c r="G309" t="s">
+        <v>588</v>
+      </c>
+      <c r="H309">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>943</v>
+      </c>
+      <c r="B310" t="s">
+        <v>600</v>
+      </c>
+      <c r="C310" t="s">
+        <v>551</v>
+      </c>
+      <c r="D310" t="s">
+        <v>601</v>
+      </c>
+      <c r="E310" t="s">
+        <v>86</v>
+      </c>
+      <c r="F310" t="s">
+        <v>87</v>
+      </c>
+      <c r="G310" t="s">
+        <v>588</v>
+      </c>
+      <c r="H310">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>944</v>
+      </c>
+      <c r="B311" t="s">
+        <v>602</v>
+      </c>
+      <c r="C311" t="s">
+        <v>554</v>
+      </c>
+      <c r="D311" t="s">
+        <v>603</v>
+      </c>
+      <c r="E311" t="s">
+        <v>86</v>
+      </c>
+      <c r="F311" t="s">
+        <v>87</v>
+      </c>
+      <c r="G311" t="s">
+        <v>588</v>
+      </c>
+      <c r="H311">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>945</v>
+      </c>
+      <c r="B312" t="s">
+        <v>604</v>
+      </c>
+      <c r="C312" t="s">
+        <v>557</v>
+      </c>
+      <c r="D312" t="s">
+        <v>605</v>
+      </c>
+      <c r="E312" t="s">
+        <v>86</v>
+      </c>
+      <c r="F312" t="s">
+        <v>87</v>
+      </c>
+      <c r="G312" t="s">
+        <v>588</v>
+      </c>
+      <c r="H312">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>946</v>
+      </c>
+      <c r="B313" t="s">
+        <v>606</v>
+      </c>
+      <c r="C313" t="s">
+        <v>560</v>
+      </c>
+      <c r="D313" t="s">
+        <v>607</v>
+      </c>
+      <c r="E313" t="s">
+        <v>86</v>
+      </c>
+      <c r="F313" t="s">
+        <v>87</v>
+      </c>
+      <c r="G313" t="s">
+        <v>588</v>
+      </c>
+      <c r="H313">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>947</v>
+      </c>
+      <c r="B314" t="s">
+        <v>608</v>
+      </c>
+      <c r="C314" t="s">
+        <v>563</v>
+      </c>
+      <c r="D314" t="s">
+        <v>609</v>
+      </c>
+      <c r="E314" t="s">
+        <v>86</v>
+      </c>
+      <c r="F314" t="s">
+        <v>87</v>
+      </c>
+      <c r="G314" t="s">
+        <v>588</v>
+      </c>
+      <c r="H314">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>948</v>
+      </c>
+      <c r="B315" t="s">
+        <v>610</v>
+      </c>
+      <c r="C315" t="s">
+        <v>566</v>
+      </c>
+      <c r="D315" t="s">
+        <v>611</v>
+      </c>
+      <c r="E315" t="s">
+        <v>86</v>
+      </c>
+      <c r="F315" t="s">
+        <v>87</v>
+      </c>
+      <c r="G315" t="s">
+        <v>588</v>
+      </c>
+      <c r="H315">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>949</v>
+      </c>
+      <c r="B316" t="s">
+        <v>612</v>
+      </c>
+      <c r="C316" t="s">
+        <v>468</v>
+      </c>
+      <c r="D316" t="s">
+        <v>469</v>
+      </c>
+      <c r="E316" t="s">
+        <v>86</v>
+      </c>
+      <c r="F316" t="s">
+        <v>87</v>
+      </c>
+      <c r="G316" t="s">
+        <v>588</v>
+      </c>
+      <c r="H316">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>950</v>
+      </c>
+      <c r="B317" t="s">
+        <v>613</v>
+      </c>
+      <c r="C317" t="s">
+        <v>571</v>
+      </c>
+      <c r="D317" t="s">
+        <v>614</v>
+      </c>
+      <c r="E317" t="s">
+        <v>86</v>
+      </c>
+      <c r="F317" t="s">
+        <v>87</v>
+      </c>
+      <c r="G317" t="s">
+        <v>588</v>
+      </c>
+      <c r="H317">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>951</v>
+      </c>
+      <c r="B318" t="s">
+        <v>615</v>
+      </c>
+      <c r="C318" t="s">
+        <v>459</v>
+      </c>
+      <c r="D318" t="s">
+        <v>460</v>
+      </c>
+      <c r="E318" t="s">
+        <v>86</v>
+      </c>
+      <c r="F318" t="s">
+        <v>87</v>
+      </c>
+      <c r="G318" t="s">
+        <v>588</v>
+      </c>
+      <c r="H318">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>952</v>
+      </c>
+      <c r="B319" t="s">
+        <v>616</v>
+      </c>
+      <c r="C319" t="s">
+        <v>576</v>
+      </c>
+      <c r="D319" t="s">
+        <v>617</v>
+      </c>
+      <c r="E319" t="s">
+        <v>86</v>
+      </c>
+      <c r="F319" t="s">
+        <v>87</v>
+      </c>
+      <c r="G319" t="s">
+        <v>588</v>
+      </c>
+      <c r="H319">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>953</v>
+      </c>
+      <c r="B320" t="s">
+        <v>618</v>
+      </c>
+      <c r="C320" t="s">
+        <v>579</v>
+      </c>
+      <c r="D320" t="s">
+        <v>619</v>
+      </c>
+      <c r="E320" t="s">
+        <v>86</v>
+      </c>
+      <c r="F320" t="s">
+        <v>87</v>
+      </c>
+      <c r="G320" t="s">
+        <v>588</v>
+      </c>
+      <c r="H320">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>954</v>
+      </c>
+      <c r="B321" t="s">
+        <v>620</v>
+      </c>
+      <c r="C321" t="s">
+        <v>582</v>
+      </c>
+      <c r="D321" t="s">
+        <v>621</v>
+      </c>
+      <c r="E321" t="s">
+        <v>86</v>
+      </c>
+      <c r="F321" t="s">
+        <v>87</v>
+      </c>
+      <c r="G321" t="s">
+        <v>588</v>
+      </c>
+      <c r="H321">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>955</v>
+      </c>
+      <c r="B322" t="s">
+        <v>622</v>
+      </c>
+      <c r="C322" t="s">
+        <v>585</v>
+      </c>
+      <c r="D322" t="s">
+        <v>623</v>
+      </c>
+      <c r="E322" t="s">
+        <v>86</v>
+      </c>
+      <c r="F322" t="s">
+        <v>87</v>
+      </c>
+      <c r="G322" t="s">
+        <v>588</v>
+      </c>
+      <c r="H322">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>956</v>
+      </c>
+      <c r="B323" t="s">
+        <v>624</v>
+      </c>
+      <c r="C323" t="s">
+        <v>420</v>
+      </c>
+      <c r="D323" t="s">
+        <v>421</v>
+      </c>
+      <c r="E323" t="s">
+        <v>86</v>
+      </c>
+      <c r="F323" t="s">
+        <v>87</v>
+      </c>
+      <c r="G323" t="s">
+        <v>625</v>
+      </c>
+      <c r="H323">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>957</v>
+      </c>
+      <c r="B324" t="s">
+        <v>626</v>
+      </c>
+      <c r="C324" t="s">
+        <v>423</v>
+      </c>
+      <c r="D324" t="s">
+        <v>424</v>
+      </c>
+      <c r="E324" t="s">
+        <v>86</v>
+      </c>
+      <c r="F324" t="s">
+        <v>87</v>
+      </c>
+      <c r="G324" t="s">
+        <v>625</v>
+      </c>
+      <c r="H324">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>958</v>
+      </c>
+      <c r="B325" t="s">
+        <v>627</v>
+      </c>
+      <c r="C325" t="s">
+        <v>536</v>
+      </c>
+      <c r="D325" t="s">
+        <v>591</v>
+      </c>
+      <c r="E325" t="s">
+        <v>86</v>
+      </c>
+      <c r="F325" t="s">
+        <v>87</v>
+      </c>
+      <c r="G325" t="s">
+        <v>625</v>
+      </c>
+      <c r="H325">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>959</v>
+      </c>
+      <c r="B326" t="s">
+        <v>628</v>
+      </c>
+      <c r="C326" t="s">
+        <v>539</v>
+      </c>
+      <c r="D326" t="s">
+        <v>593</v>
+      </c>
+      <c r="E326" t="s">
+        <v>86</v>
+      </c>
+      <c r="F326" t="s">
+        <v>87</v>
+      </c>
+      <c r="G326" t="s">
+        <v>625</v>
+      </c>
+      <c r="H326">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>960</v>
+      </c>
+      <c r="B327" t="s">
+        <v>629</v>
+      </c>
+      <c r="C327" t="s">
+        <v>542</v>
+      </c>
+      <c r="D327" t="s">
+        <v>595</v>
+      </c>
+      <c r="E327" t="s">
+        <v>86</v>
+      </c>
+      <c r="F327" t="s">
+        <v>87</v>
+      </c>
+      <c r="G327" t="s">
+        <v>625</v>
+      </c>
+      <c r="H327">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>961</v>
+      </c>
+      <c r="B328" t="s">
+        <v>630</v>
+      </c>
+      <c r="C328" t="s">
+        <v>545</v>
+      </c>
+      <c r="D328" t="s">
+        <v>597</v>
+      </c>
+      <c r="E328" t="s">
+        <v>86</v>
+      </c>
+      <c r="F328" t="s">
+        <v>87</v>
+      </c>
+      <c r="G328" t="s">
+        <v>625</v>
+      </c>
+      <c r="H328">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>962</v>
+      </c>
+      <c r="B329" t="s">
+        <v>631</v>
+      </c>
+      <c r="C329" t="s">
+        <v>548</v>
+      </c>
+      <c r="D329" t="s">
+        <v>599</v>
+      </c>
+      <c r="E329" t="s">
+        <v>86</v>
+      </c>
+      <c r="F329" t="s">
+        <v>87</v>
+      </c>
+      <c r="G329" t="s">
+        <v>625</v>
+      </c>
+      <c r="H329">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>963</v>
+      </c>
+      <c r="B330" t="s">
+        <v>632</v>
+      </c>
+      <c r="C330" t="s">
+        <v>551</v>
+      </c>
+      <c r="D330" t="s">
+        <v>601</v>
+      </c>
+      <c r="E330" t="s">
+        <v>86</v>
+      </c>
+      <c r="F330" t="s">
+        <v>87</v>
+      </c>
+      <c r="G330" t="s">
+        <v>625</v>
+      </c>
+      <c r="H330">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>964</v>
+      </c>
+      <c r="B331" t="s">
+        <v>633</v>
+      </c>
+      <c r="C331" t="s">
+        <v>554</v>
+      </c>
+      <c r="D331" t="s">
+        <v>603</v>
+      </c>
+      <c r="E331" t="s">
+        <v>86</v>
+      </c>
+      <c r="F331" t="s">
+        <v>87</v>
+      </c>
+      <c r="G331" t="s">
+        <v>625</v>
+      </c>
+      <c r="H331">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>965</v>
+      </c>
+      <c r="B332" t="s">
+        <v>634</v>
+      </c>
+      <c r="C332" t="s">
+        <v>557</v>
+      </c>
+      <c r="D332" t="s">
+        <v>605</v>
+      </c>
+      <c r="E332" t="s">
+        <v>86</v>
+      </c>
+      <c r="F332" t="s">
+        <v>87</v>
+      </c>
+      <c r="G332" t="s">
+        <v>625</v>
+      </c>
+      <c r="H332">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>966</v>
+      </c>
+      <c r="B333" t="s">
+        <v>635</v>
+      </c>
+      <c r="C333" t="s">
+        <v>560</v>
+      </c>
+      <c r="D333" t="s">
+        <v>607</v>
+      </c>
+      <c r="E333" t="s">
+        <v>86</v>
+      </c>
+      <c r="F333" t="s">
+        <v>87</v>
+      </c>
+      <c r="G333" t="s">
+        <v>625</v>
+      </c>
+      <c r="H333">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>967</v>
+      </c>
+      <c r="B334" t="s">
+        <v>636</v>
+      </c>
+      <c r="C334" t="s">
+        <v>563</v>
+      </c>
+      <c r="D334" t="s">
+        <v>609</v>
+      </c>
+      <c r="E334" t="s">
+        <v>86</v>
+      </c>
+      <c r="F334" t="s">
+        <v>87</v>
+      </c>
+      <c r="G334" t="s">
+        <v>625</v>
+      </c>
+      <c r="H334">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>968</v>
+      </c>
+      <c r="B335" t="s">
+        <v>637</v>
+      </c>
+      <c r="C335" t="s">
+        <v>566</v>
+      </c>
+      <c r="D335" t="s">
+        <v>611</v>
+      </c>
+      <c r="E335" t="s">
+        <v>86</v>
+      </c>
+      <c r="F335" t="s">
+        <v>87</v>
+      </c>
+      <c r="G335" t="s">
+        <v>625</v>
+      </c>
+      <c r="H335">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>969</v>
+      </c>
+      <c r="B336" t="s">
+        <v>638</v>
+      </c>
+      <c r="C336" t="s">
+        <v>468</v>
+      </c>
+      <c r="D336" t="s">
+        <v>469</v>
+      </c>
+      <c r="E336" t="s">
+        <v>86</v>
+      </c>
+      <c r="F336" t="s">
+        <v>87</v>
+      </c>
+      <c r="G336" t="s">
+        <v>625</v>
+      </c>
+      <c r="H336">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>970</v>
+      </c>
+      <c r="B337" t="s">
+        <v>639</v>
+      </c>
+      <c r="C337" t="s">
+        <v>571</v>
+      </c>
+      <c r="D337" t="s">
+        <v>614</v>
+      </c>
+      <c r="E337" t="s">
+        <v>86</v>
+      </c>
+      <c r="F337" t="s">
+        <v>87</v>
+      </c>
+      <c r="G337" t="s">
+        <v>625</v>
+      </c>
+      <c r="H337">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>971</v>
+      </c>
+      <c r="B338" t="s">
+        <v>640</v>
+      </c>
+      <c r="C338" t="s">
+        <v>459</v>
+      </c>
+      <c r="D338" t="s">
+        <v>460</v>
+      </c>
+      <c r="E338" t="s">
+        <v>86</v>
+      </c>
+      <c r="F338" t="s">
+        <v>87</v>
+      </c>
+      <c r="G338" t="s">
+        <v>625</v>
+      </c>
+      <c r="H338">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>972</v>
+      </c>
+      <c r="B339" t="s">
+        <v>641</v>
+      </c>
+      <c r="C339" t="s">
+        <v>576</v>
+      </c>
+      <c r="D339" t="s">
+        <v>617</v>
+      </c>
+      <c r="E339" t="s">
+        <v>86</v>
+      </c>
+      <c r="F339" t="s">
+        <v>87</v>
+      </c>
+      <c r="G339" t="s">
+        <v>625</v>
+      </c>
+      <c r="H339">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>973</v>
+      </c>
+      <c r="B340" t="s">
+        <v>642</v>
+      </c>
+      <c r="C340" t="s">
+        <v>579</v>
+      </c>
+      <c r="D340" t="s">
+        <v>619</v>
+      </c>
+      <c r="E340" t="s">
+        <v>86</v>
+      </c>
+      <c r="F340" t="s">
+        <v>87</v>
+      </c>
+      <c r="G340" t="s">
+        <v>625</v>
+      </c>
+      <c r="H340">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>974</v>
+      </c>
+      <c r="B341" t="s">
+        <v>643</v>
+      </c>
+      <c r="C341" t="s">
+        <v>582</v>
+      </c>
+      <c r="D341" t="s">
+        <v>621</v>
+      </c>
+      <c r="E341" t="s">
+        <v>86</v>
+      </c>
+      <c r="F341" t="s">
+        <v>87</v>
+      </c>
+      <c r="G341" t="s">
+        <v>625</v>
+      </c>
+      <c r="H341">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>975</v>
+      </c>
+      <c r="B342" t="s">
+        <v>644</v>
+      </c>
+      <c r="C342" t="s">
+        <v>585</v>
+      </c>
+      <c r="D342" t="s">
+        <v>623</v>
+      </c>
+      <c r="E342" t="s">
+        <v>86</v>
+      </c>
+      <c r="F342" t="s">
+        <v>87</v>
+      </c>
+      <c r="G342" t="s">
+        <v>625</v>
+      </c>
+      <c r="H342">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>976</v>
+      </c>
+      <c r="B343" t="s">
+        <v>645</v>
+      </c>
+      <c r="C343" t="s">
+        <v>646</v>
+      </c>
+      <c r="D343" t="s">
+        <v>647</v>
+      </c>
+      <c r="E343" t="s">
+        <v>86</v>
+      </c>
+      <c r="F343" t="s">
+        <v>87</v>
+      </c>
+      <c r="G343" t="s">
+        <v>648</v>
+      </c>
+      <c r="H343">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>977</v>
+      </c>
+      <c r="B344" t="s">
+        <v>481</v>
+      </c>
+      <c r="C344" t="s">
+        <v>649</v>
+      </c>
+      <c r="D344" t="s">
+        <v>650</v>
+      </c>
+      <c r="E344" t="s">
+        <v>86</v>
+      </c>
+      <c r="F344" t="s">
+        <v>87</v>
+      </c>
+      <c r="G344" t="s">
+        <v>648</v>
+      </c>
+      <c r="H344">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>978</v>
+      </c>
+      <c r="B345" t="s">
+        <v>651</v>
+      </c>
+      <c r="C345" t="s">
+        <v>536</v>
+      </c>
+      <c r="D345" t="s">
+        <v>652</v>
+      </c>
+      <c r="E345" t="s">
+        <v>86</v>
+      </c>
+      <c r="F345" t="s">
+        <v>87</v>
+      </c>
+      <c r="G345" t="s">
+        <v>648</v>
+      </c>
+      <c r="H345">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>979</v>
+      </c>
+      <c r="B346" t="s">
+        <v>653</v>
+      </c>
+      <c r="C346" t="s">
+        <v>654</v>
+      </c>
+      <c r="D346" t="s">
+        <v>655</v>
+      </c>
+      <c r="E346" t="s">
+        <v>86</v>
+      </c>
+      <c r="F346" t="s">
+        <v>87</v>
+      </c>
+      <c r="G346" t="s">
+        <v>648</v>
+      </c>
+      <c r="H346">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>980</v>
+      </c>
+      <c r="B347" t="s">
+        <v>656</v>
+      </c>
+      <c r="C347" t="s">
+        <v>542</v>
+      </c>
+      <c r="D347" t="s">
+        <v>543</v>
+      </c>
+      <c r="E347" t="s">
+        <v>86</v>
+      </c>
+      <c r="F347" t="s">
+        <v>87</v>
+      </c>
+      <c r="G347" t="s">
+        <v>648</v>
+      </c>
+      <c r="H347">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>981</v>
+      </c>
+      <c r="B348" t="s">
+        <v>657</v>
+      </c>
+      <c r="C348" t="s">
+        <v>658</v>
+      </c>
+      <c r="D348" t="s">
+        <v>659</v>
+      </c>
+      <c r="E348" t="s">
+        <v>86</v>
+      </c>
+      <c r="F348" t="s">
+        <v>87</v>
+      </c>
+      <c r="G348" t="s">
+        <v>648</v>
+      </c>
+      <c r="H348">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>982</v>
+      </c>
+      <c r="B349" t="s">
+        <v>660</v>
+      </c>
+      <c r="C349" t="s">
+        <v>661</v>
+      </c>
+      <c r="D349" t="s">
+        <v>549</v>
+      </c>
+      <c r="E349" t="s">
+        <v>86</v>
+      </c>
+      <c r="F349" t="s">
+        <v>87</v>
+      </c>
+      <c r="G349" t="s">
+        <v>648</v>
+      </c>
+      <c r="H349">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>983</v>
+      </c>
+      <c r="B350" t="s">
+        <v>662</v>
+      </c>
+      <c r="C350" t="s">
+        <v>663</v>
+      </c>
+      <c r="D350" t="s">
+        <v>664</v>
+      </c>
+      <c r="E350" t="s">
+        <v>86</v>
+      </c>
+      <c r="F350" t="s">
+        <v>87</v>
+      </c>
+      <c r="G350" t="s">
+        <v>648</v>
+      </c>
+      <c r="H350">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>984</v>
+      </c>
+      <c r="B351" t="s">
+        <v>665</v>
+      </c>
+      <c r="C351" t="s">
+        <v>554</v>
+      </c>
+      <c r="D351" t="s">
+        <v>555</v>
+      </c>
+      <c r="E351" t="s">
+        <v>86</v>
+      </c>
+      <c r="F351" t="s">
+        <v>87</v>
+      </c>
+      <c r="G351" t="s">
+        <v>648</v>
+      </c>
+      <c r="H351">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>985</v>
+      </c>
+      <c r="B352" t="s">
+        <v>666</v>
+      </c>
+      <c r="C352" t="s">
+        <v>557</v>
+      </c>
+      <c r="D352" t="s">
+        <v>558</v>
+      </c>
+      <c r="E352" t="s">
+        <v>86</v>
+      </c>
+      <c r="F352" t="s">
+        <v>87</v>
+      </c>
+      <c r="G352" t="s">
+        <v>648</v>
+      </c>
+      <c r="H352">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>986</v>
+      </c>
+      <c r="B353" t="s">
+        <v>667</v>
+      </c>
+      <c r="C353" t="s">
+        <v>668</v>
+      </c>
+      <c r="D353" t="s">
+        <v>669</v>
+      </c>
+      <c r="E353" t="s">
+        <v>86</v>
+      </c>
+      <c r="F353" t="s">
+        <v>87</v>
+      </c>
+      <c r="G353" t="s">
+        <v>648</v>
+      </c>
+      <c r="H353">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>987</v>
+      </c>
+      <c r="B354" t="s">
+        <v>670</v>
+      </c>
+      <c r="C354" t="s">
+        <v>563</v>
+      </c>
+      <c r="D354" t="s">
+        <v>671</v>
+      </c>
+      <c r="E354" t="s">
+        <v>86</v>
+      </c>
+      <c r="F354" t="s">
+        <v>87</v>
+      </c>
+      <c r="G354" t="s">
+        <v>648</v>
+      </c>
+      <c r="H354">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>988</v>
+      </c>
+      <c r="B355" t="s">
+        <v>672</v>
+      </c>
+      <c r="C355" t="s">
+        <v>485</v>
+      </c>
+      <c r="D355" t="s">
+        <v>673</v>
+      </c>
+      <c r="E355" t="s">
+        <v>86</v>
+      </c>
+      <c r="F355" t="s">
+        <v>87</v>
+      </c>
+      <c r="G355" t="s">
+        <v>648</v>
+      </c>
+      <c r="H355">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>989</v>
+      </c>
+      <c r="B356" t="s">
+        <v>674</v>
+      </c>
+      <c r="C356" t="s">
+        <v>435</v>
+      </c>
+      <c r="D356" t="s">
+        <v>569</v>
+      </c>
+      <c r="E356" t="s">
+        <v>86</v>
+      </c>
+      <c r="F356" t="s">
+        <v>87</v>
+      </c>
+      <c r="G356" t="s">
+        <v>648</v>
+      </c>
+      <c r="H356">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>990</v>
+      </c>
+      <c r="B357" t="s">
+        <v>479</v>
+      </c>
+      <c r="C357" t="s">
+        <v>444</v>
+      </c>
+      <c r="D357" t="s">
+        <v>675</v>
+      </c>
+      <c r="E357" t="s">
+        <v>86</v>
+      </c>
+      <c r="F357" t="s">
+        <v>87</v>
+      </c>
+      <c r="G357" t="s">
+        <v>648</v>
+      </c>
+      <c r="H357">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>991</v>
+      </c>
+      <c r="B358" t="s">
+        <v>676</v>
+      </c>
+      <c r="C358" t="s">
+        <v>677</v>
+      </c>
+      <c r="D358" t="s">
+        <v>678</v>
+      </c>
+      <c r="E358" t="s">
+        <v>86</v>
+      </c>
+      <c r="F358" t="s">
+        <v>87</v>
+      </c>
+      <c r="G358" t="s">
+        <v>648</v>
+      </c>
+      <c r="H358">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>992</v>
+      </c>
+      <c r="B359" t="s">
+        <v>679</v>
+      </c>
+      <c r="C359" t="s">
+        <v>576</v>
+      </c>
+      <c r="D359" t="s">
+        <v>577</v>
+      </c>
+      <c r="E359" t="s">
+        <v>86</v>
+      </c>
+      <c r="F359" t="s">
+        <v>87</v>
+      </c>
+      <c r="G359" t="s">
+        <v>648</v>
+      </c>
+      <c r="H359">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>993</v>
+      </c>
+      <c r="B360" t="s">
+        <v>680</v>
+      </c>
+      <c r="C360" t="s">
+        <v>579</v>
+      </c>
+      <c r="D360" t="s">
+        <v>681</v>
+      </c>
+      <c r="E360" t="s">
+        <v>86</v>
+      </c>
+      <c r="F360" t="s">
+        <v>87</v>
+      </c>
+      <c r="G360" t="s">
+        <v>648</v>
+      </c>
+      <c r="H360">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>994</v>
+      </c>
+      <c r="B361" t="s">
+        <v>682</v>
+      </c>
+      <c r="C361" t="s">
+        <v>582</v>
+      </c>
+      <c r="D361" t="s">
+        <v>583</v>
+      </c>
+      <c r="E361" t="s">
+        <v>86</v>
+      </c>
+      <c r="F361" t="s">
+        <v>87</v>
+      </c>
+      <c r="G361" t="s">
+        <v>648</v>
+      </c>
+      <c r="H361">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>995</v>
+      </c>
+      <c r="B362" t="s">
+        <v>683</v>
+      </c>
+      <c r="C362" t="s">
+        <v>684</v>
+      </c>
+      <c r="D362" t="s">
+        <v>685</v>
+      </c>
+      <c r="E362" t="s">
+        <v>86</v>
+      </c>
+      <c r="F362" t="s">
+        <v>87</v>
+      </c>
+      <c r="G362" t="s">
+        <v>648</v>
+      </c>
+      <c r="H362">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>996</v>
+      </c>
+      <c r="B363" t="s">
+        <v>686</v>
+      </c>
+      <c r="C363" t="s">
+        <v>687</v>
+      </c>
+      <c r="D363" t="s">
+        <v>688</v>
+      </c>
+      <c r="E363" t="s">
+        <v>86</v>
+      </c>
+      <c r="F363" t="s">
+        <v>87</v>
+      </c>
+      <c r="G363" t="s">
+        <v>689</v>
+      </c>
+      <c r="H363">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>997</v>
+      </c>
+      <c r="B364" t="s">
+        <v>690</v>
+      </c>
+      <c r="C364" t="s">
+        <v>691</v>
+      </c>
+      <c r="D364" t="s">
+        <v>692</v>
+      </c>
+      <c r="E364" t="s">
+        <v>86</v>
+      </c>
+      <c r="F364" t="s">
+        <v>87</v>
+      </c>
+      <c r="G364" t="s">
+        <v>689</v>
+      </c>
+      <c r="H364">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>998</v>
+      </c>
+      <c r="B365" t="s">
+        <v>693</v>
+      </c>
+      <c r="C365" t="s">
+        <v>694</v>
+      </c>
+      <c r="D365" t="s">
+        <v>695</v>
+      </c>
+      <c r="E365" t="s">
+        <v>86</v>
+      </c>
+      <c r="F365" t="s">
+        <v>87</v>
+      </c>
+      <c r="G365" t="s">
+        <v>689</v>
+      </c>
+      <c r="H365">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>999</v>
+      </c>
+      <c r="B366" t="s">
+        <v>696</v>
+      </c>
+      <c r="C366" t="s">
+        <v>697</v>
+      </c>
+      <c r="D366" t="s">
+        <v>698</v>
+      </c>
+      <c r="E366" t="s">
+        <v>86</v>
+      </c>
+      <c r="F366" t="s">
+        <v>87</v>
+      </c>
+      <c r="G366" t="s">
+        <v>689</v>
+      </c>
+      <c r="H366">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B367" t="s">
+        <v>699</v>
+      </c>
+      <c r="C367" t="s">
+        <v>435</v>
+      </c>
+      <c r="D367" t="s">
+        <v>700</v>
+      </c>
+      <c r="E367" t="s">
+        <v>86</v>
+      </c>
+      <c r="F367" t="s">
+        <v>87</v>
+      </c>
+      <c r="G367" t="s">
+        <v>689</v>
+      </c>
+      <c r="H367">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B368" t="s">
+        <v>701</v>
+      </c>
+      <c r="C368" t="s">
+        <v>702</v>
+      </c>
+      <c r="D368" t="s">
+        <v>703</v>
+      </c>
+      <c r="E368" t="s">
+        <v>86</v>
+      </c>
+      <c r="F368" t="s">
+        <v>87</v>
+      </c>
+      <c r="G368" t="s">
+        <v>689</v>
+      </c>
+      <c r="H368">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B369" t="s">
+        <v>704</v>
+      </c>
+      <c r="C369" t="s">
+        <v>661</v>
+      </c>
+      <c r="D369" t="s">
+        <v>705</v>
+      </c>
+      <c r="E369" t="s">
+        <v>86</v>
+      </c>
+      <c r="F369" t="s">
+        <v>87</v>
+      </c>
+      <c r="G369" t="s">
+        <v>689</v>
+      </c>
+      <c r="H369">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B370" t="s">
+        <v>706</v>
+      </c>
+      <c r="C370" t="s">
+        <v>663</v>
+      </c>
+      <c r="D370" t="s">
+        <v>707</v>
+      </c>
+      <c r="E370" t="s">
+        <v>86</v>
+      </c>
+      <c r="F370" t="s">
+        <v>87</v>
+      </c>
+      <c r="G370" t="s">
+        <v>689</v>
+      </c>
+      <c r="H370">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B371" t="s">
+        <v>708</v>
+      </c>
+      <c r="C371" t="s">
+        <v>709</v>
+      </c>
+      <c r="D371" t="s">
+        <v>710</v>
+      </c>
+      <c r="E371" t="s">
+        <v>86</v>
+      </c>
+      <c r="F371" t="s">
+        <v>87</v>
+      </c>
+      <c r="G371" t="s">
+        <v>689</v>
+      </c>
+      <c r="H371">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B372" t="s">
+        <v>711</v>
+      </c>
+      <c r="C372" t="s">
+        <v>557</v>
+      </c>
+      <c r="D372" t="s">
+        <v>712</v>
+      </c>
+      <c r="E372" t="s">
+        <v>86</v>
+      </c>
+      <c r="F372" t="s">
+        <v>87</v>
+      </c>
+      <c r="G372" t="s">
+        <v>689</v>
+      </c>
+      <c r="H372">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B373" t="s">
+        <v>713</v>
+      </c>
+      <c r="C373" t="s">
+        <v>714</v>
+      </c>
+      <c r="D373" t="s">
+        <v>715</v>
+      </c>
+      <c r="E373" t="s">
+        <v>86</v>
+      </c>
+      <c r="F373" t="s">
+        <v>87</v>
+      </c>
+      <c r="G373" t="s">
+        <v>689</v>
+      </c>
+      <c r="H373">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B374" t="s">
+        <v>716</v>
+      </c>
+      <c r="C374" t="s">
+        <v>563</v>
+      </c>
+      <c r="D374" t="s">
+        <v>717</v>
+      </c>
+      <c r="E374" t="s">
+        <v>86</v>
+      </c>
+      <c r="F374" t="s">
+        <v>87</v>
+      </c>
+      <c r="G374" t="s">
+        <v>689</v>
+      </c>
+      <c r="H374">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B375" t="s">
+        <v>718</v>
+      </c>
+      <c r="C375" t="s">
+        <v>719</v>
+      </c>
+      <c r="D375" t="s">
+        <v>720</v>
+      </c>
+      <c r="E375" t="s">
+        <v>86</v>
+      </c>
+      <c r="F375" t="s">
+        <v>87</v>
+      </c>
+      <c r="G375" t="s">
+        <v>689</v>
+      </c>
+      <c r="H375">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B376" t="s">
+        <v>721</v>
+      </c>
+      <c r="C376" t="s">
+        <v>528</v>
+      </c>
+      <c r="D376" t="s">
+        <v>722</v>
+      </c>
+      <c r="E376" t="s">
+        <v>86</v>
+      </c>
+      <c r="F376" t="s">
+        <v>87</v>
+      </c>
+      <c r="G376" t="s">
+        <v>689</v>
+      </c>
+      <c r="H376">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B377" t="s">
+        <v>723</v>
+      </c>
+      <c r="C377" t="s">
+        <v>459</v>
+      </c>
+      <c r="D377" t="s">
+        <v>724</v>
+      </c>
+      <c r="E377" t="s">
+        <v>86</v>
+      </c>
+      <c r="F377" t="s">
+        <v>87</v>
+      </c>
+      <c r="G377" t="s">
+        <v>689</v>
+      </c>
+      <c r="H377">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B378" t="s">
+        <v>725</v>
+      </c>
+      <c r="C378" t="s">
+        <v>726</v>
+      </c>
+      <c r="D378" t="s">
+        <v>727</v>
+      </c>
+      <c r="E378" t="s">
+        <v>86</v>
+      </c>
+      <c r="F378" t="s">
+        <v>87</v>
+      </c>
+      <c r="G378" t="s">
+        <v>689</v>
+      </c>
+      <c r="H378">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B379" t="s">
+        <v>728</v>
+      </c>
+      <c r="C379" t="s">
+        <v>444</v>
+      </c>
+      <c r="D379" t="s">
+        <v>729</v>
+      </c>
+      <c r="E379" t="s">
+        <v>86</v>
+      </c>
+      <c r="F379" t="s">
+        <v>87</v>
+      </c>
+      <c r="G379" t="s">
+        <v>689</v>
+      </c>
+      <c r="H379">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B380" t="s">
+        <v>716</v>
+      </c>
+      <c r="C380" t="s">
+        <v>563</v>
+      </c>
+      <c r="D380" t="s">
+        <v>717</v>
+      </c>
+      <c r="E380" t="s">
+        <v>86</v>
+      </c>
+      <c r="F380" t="s">
+        <v>87</v>
+      </c>
+      <c r="G380" t="s">
+        <v>689</v>
+      </c>
+      <c r="H380">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B381" t="s">
+        <v>730</v>
+      </c>
+      <c r="C381" t="s">
+        <v>731</v>
+      </c>
+      <c r="D381" t="s">
+        <v>732</v>
+      </c>
+      <c r="E381" t="s">
+        <v>86</v>
+      </c>
+      <c r="F381" t="s">
+        <v>87</v>
+      </c>
+      <c r="G381" t="s">
+        <v>689</v>
+      </c>
+      <c r="H381">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B382" t="s">
+        <v>733</v>
+      </c>
+      <c r="C382" t="s">
+        <v>734</v>
+      </c>
+      <c r="D382" t="s">
+        <v>735</v>
+      </c>
+      <c r="E382" t="s">
+        <v>86</v>
+      </c>
+      <c r="F382" t="s">
+        <v>87</v>
+      </c>
+      <c r="G382" t="s">
+        <v>689</v>
+      </c>
+      <c r="H382">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added code for french
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\Desktop\langapp\v17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\Desktop\langapp\v19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA28D49E-39CF-4C96-B0EB-BD28B6F651FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34931218-691A-4A44-B74E-1A388364875D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7340545C-2BB6-4E8B-827D-6673ABB13FB9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{7340545C-2BB6-4E8B-827D-6673ABB13FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2880" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3860" uniqueCount="1156">
   <si>
     <t>question_text</t>
   </si>
@@ -3085,6 +3085,426 @@
   </si>
   <si>
     <t>160. German question</t>
+  </si>
+  <si>
+    <t>21. French question</t>
+  </si>
+  <si>
+    <t>22. French question</t>
+  </si>
+  <si>
+    <t>23. French question</t>
+  </si>
+  <si>
+    <t>24. French question</t>
+  </si>
+  <si>
+    <t>25. French question</t>
+  </si>
+  <si>
+    <t>26. French question</t>
+  </si>
+  <si>
+    <t>27. French question</t>
+  </si>
+  <si>
+    <t>28. French question</t>
+  </si>
+  <si>
+    <t>29. French question</t>
+  </si>
+  <si>
+    <t>30. French question</t>
+  </si>
+  <si>
+    <t>31. French question</t>
+  </si>
+  <si>
+    <t>32. French question</t>
+  </si>
+  <si>
+    <t>33. French question</t>
+  </si>
+  <si>
+    <t>34. French question</t>
+  </si>
+  <si>
+    <t>35. French question</t>
+  </si>
+  <si>
+    <t>36. French question</t>
+  </si>
+  <si>
+    <t>37. French question</t>
+  </si>
+  <si>
+    <t>38. French question</t>
+  </si>
+  <si>
+    <t>39. French question</t>
+  </si>
+  <si>
+    <t>40. French question</t>
+  </si>
+  <si>
+    <t>41. French question</t>
+  </si>
+  <si>
+    <t>42. French question</t>
+  </si>
+  <si>
+    <t>43. French question</t>
+  </si>
+  <si>
+    <t>44. French question</t>
+  </si>
+  <si>
+    <t>45. French question</t>
+  </si>
+  <si>
+    <t>46. French question</t>
+  </si>
+  <si>
+    <t>47. French question</t>
+  </si>
+  <si>
+    <t>48. French question</t>
+  </si>
+  <si>
+    <t>49. French question</t>
+  </si>
+  <si>
+    <t>50. French question</t>
+  </si>
+  <si>
+    <t>51. French question</t>
+  </si>
+  <si>
+    <t>52. French question</t>
+  </si>
+  <si>
+    <t>53. French question</t>
+  </si>
+  <si>
+    <t>54. French question</t>
+  </si>
+  <si>
+    <t>55. French question</t>
+  </si>
+  <si>
+    <t>56. French question</t>
+  </si>
+  <si>
+    <t>57. French question</t>
+  </si>
+  <si>
+    <t>58. French question</t>
+  </si>
+  <si>
+    <t>59. French question</t>
+  </si>
+  <si>
+    <t>60. French question</t>
+  </si>
+  <si>
+    <t>61. French question</t>
+  </si>
+  <si>
+    <t>62. French question</t>
+  </si>
+  <si>
+    <t>63. French question</t>
+  </si>
+  <si>
+    <t>64. French question</t>
+  </si>
+  <si>
+    <t>65. French question</t>
+  </si>
+  <si>
+    <t>66. French question</t>
+  </si>
+  <si>
+    <t>67. French question</t>
+  </si>
+  <si>
+    <t>68. French question</t>
+  </si>
+  <si>
+    <t>69. French question</t>
+  </si>
+  <si>
+    <t>70. French question</t>
+  </si>
+  <si>
+    <t>71. French question</t>
+  </si>
+  <si>
+    <t>72. French question</t>
+  </si>
+  <si>
+    <t>73. French question</t>
+  </si>
+  <si>
+    <t>74. French question</t>
+  </si>
+  <si>
+    <t>75. French question</t>
+  </si>
+  <si>
+    <t>76. French question</t>
+  </si>
+  <si>
+    <t>77. French question</t>
+  </si>
+  <si>
+    <t>78. French question</t>
+  </si>
+  <si>
+    <t>79. French question</t>
+  </si>
+  <si>
+    <t>80. French question</t>
+  </si>
+  <si>
+    <t>81. French question</t>
+  </si>
+  <si>
+    <t>82. French question</t>
+  </si>
+  <si>
+    <t>83. French question</t>
+  </si>
+  <si>
+    <t>84. French question</t>
+  </si>
+  <si>
+    <t>85. French question</t>
+  </si>
+  <si>
+    <t>86. French question</t>
+  </si>
+  <si>
+    <t>87. French question</t>
+  </si>
+  <si>
+    <t>88. French question</t>
+  </si>
+  <si>
+    <t>89. French question</t>
+  </si>
+  <si>
+    <t>90. French question</t>
+  </si>
+  <si>
+    <t>91. French question</t>
+  </si>
+  <si>
+    <t>92. French question</t>
+  </si>
+  <si>
+    <t>93. French question</t>
+  </si>
+  <si>
+    <t>94. French question</t>
+  </si>
+  <si>
+    <t>95. French question</t>
+  </si>
+  <si>
+    <t>96. French question</t>
+  </si>
+  <si>
+    <t>97. French question</t>
+  </si>
+  <si>
+    <t>98. French question</t>
+  </si>
+  <si>
+    <t>99. French question</t>
+  </si>
+  <si>
+    <t>100. French question</t>
+  </si>
+  <si>
+    <t>101. French question</t>
+  </si>
+  <si>
+    <t>102. French question</t>
+  </si>
+  <si>
+    <t>103. French question</t>
+  </si>
+  <si>
+    <t>104. French question</t>
+  </si>
+  <si>
+    <t>105. French question</t>
+  </si>
+  <si>
+    <t>106. French question</t>
+  </si>
+  <si>
+    <t>107. French question</t>
+  </si>
+  <si>
+    <t>108. French question</t>
+  </si>
+  <si>
+    <t>109. French question</t>
+  </si>
+  <si>
+    <t>110. French question</t>
+  </si>
+  <si>
+    <t>111. French question</t>
+  </si>
+  <si>
+    <t>112. French question</t>
+  </si>
+  <si>
+    <t>113. French question</t>
+  </si>
+  <si>
+    <t>114. French question</t>
+  </si>
+  <si>
+    <t>115. French question</t>
+  </si>
+  <si>
+    <t>116. French question</t>
+  </si>
+  <si>
+    <t>117. French question</t>
+  </si>
+  <si>
+    <t>118. French question</t>
+  </si>
+  <si>
+    <t>119. French question</t>
+  </si>
+  <si>
+    <t>120. French question</t>
+  </si>
+  <si>
+    <t>121. French question</t>
+  </si>
+  <si>
+    <t>122. French question</t>
+  </si>
+  <si>
+    <t>123. French question</t>
+  </si>
+  <si>
+    <t>124. French question</t>
+  </si>
+  <si>
+    <t>125. French question</t>
+  </si>
+  <si>
+    <t>126. French question</t>
+  </si>
+  <si>
+    <t>127. French question</t>
+  </si>
+  <si>
+    <t>128. French question</t>
+  </si>
+  <si>
+    <t>129. French question</t>
+  </si>
+  <si>
+    <t>130. French question</t>
+  </si>
+  <si>
+    <t>131. French question</t>
+  </si>
+  <si>
+    <t>132. French question</t>
+  </si>
+  <si>
+    <t>133. French question</t>
+  </si>
+  <si>
+    <t>134. French question</t>
+  </si>
+  <si>
+    <t>135. French question</t>
+  </si>
+  <si>
+    <t>136. French question</t>
+  </si>
+  <si>
+    <t>137. French question</t>
+  </si>
+  <si>
+    <t>138. French question</t>
+  </si>
+  <si>
+    <t>139. French question</t>
+  </si>
+  <si>
+    <t>140. French question</t>
+  </si>
+  <si>
+    <t>141. French question</t>
+  </si>
+  <si>
+    <t>142. French question</t>
+  </si>
+  <si>
+    <t>143. French question</t>
+  </si>
+  <si>
+    <t>144. French question</t>
+  </si>
+  <si>
+    <t>145. French question</t>
+  </si>
+  <si>
+    <t>146. French question</t>
+  </si>
+  <si>
+    <t>147. French question</t>
+  </si>
+  <si>
+    <t>148. French question</t>
+  </si>
+  <si>
+    <t>149. French question</t>
+  </si>
+  <si>
+    <t>150. French question</t>
+  </si>
+  <si>
+    <t>151. French question</t>
+  </si>
+  <si>
+    <t>152. French question</t>
+  </si>
+  <si>
+    <t>153. French question</t>
+  </si>
+  <si>
+    <t>154. French question</t>
+  </si>
+  <si>
+    <t>155. French question</t>
+  </si>
+  <si>
+    <t>156. French question</t>
+  </si>
+  <si>
+    <t>157. French question</t>
+  </si>
+  <si>
+    <t>158. French question</t>
+  </si>
+  <si>
+    <t>159. French question</t>
+  </si>
+  <si>
+    <t>160. French question</t>
   </si>
 </sst>
 </file>
@@ -3443,10 +3863,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36A3347-166D-4930-B9BE-A2A96E4C6F8D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H382"/>
+  <dimension ref="A1:H522"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="J243" sqref="J243"/>
+    <sheetView tabSelected="1" topLeftCell="A487" workbookViewId="0">
+      <selection activeCell="A522" sqref="A522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13383,6 +13803,3646 @@
         <v>689</v>
       </c>
       <c r="H382">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B383" t="s">
+        <v>419</v>
+      </c>
+      <c r="C383" t="s">
+        <v>420</v>
+      </c>
+      <c r="D383" t="s">
+        <v>421</v>
+      </c>
+      <c r="E383" t="s">
+        <v>86</v>
+      </c>
+      <c r="F383" t="s">
+        <v>166</v>
+      </c>
+      <c r="G383" t="s">
+        <v>408</v>
+      </c>
+      <c r="H383">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B384" t="s">
+        <v>422</v>
+      </c>
+      <c r="C384" t="s">
+        <v>423</v>
+      </c>
+      <c r="D384" t="s">
+        <v>424</v>
+      </c>
+      <c r="E384" t="s">
+        <v>86</v>
+      </c>
+      <c r="F384" t="s">
+        <v>166</v>
+      </c>
+      <c r="G384" t="s">
+        <v>408</v>
+      </c>
+      <c r="H384">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B385" t="s">
+        <v>425</v>
+      </c>
+      <c r="C385" t="s">
+        <v>426</v>
+      </c>
+      <c r="D385" t="s">
+        <v>427</v>
+      </c>
+      <c r="E385" t="s">
+        <v>86</v>
+      </c>
+      <c r="F385" t="s">
+        <v>166</v>
+      </c>
+      <c r="G385" t="s">
+        <v>408</v>
+      </c>
+      <c r="H385">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B386" t="s">
+        <v>428</v>
+      </c>
+      <c r="C386" t="s">
+        <v>429</v>
+      </c>
+      <c r="D386" t="s">
+        <v>430</v>
+      </c>
+      <c r="E386" t="s">
+        <v>86</v>
+      </c>
+      <c r="F386" t="s">
+        <v>166</v>
+      </c>
+      <c r="G386" t="s">
+        <v>408</v>
+      </c>
+      <c r="H386">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B387" t="s">
+        <v>431</v>
+      </c>
+      <c r="C387" t="s">
+        <v>432</v>
+      </c>
+      <c r="D387" t="s">
+        <v>433</v>
+      </c>
+      <c r="E387" t="s">
+        <v>86</v>
+      </c>
+      <c r="F387" t="s">
+        <v>166</v>
+      </c>
+      <c r="G387" t="s">
+        <v>408</v>
+      </c>
+      <c r="H387">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B388" t="s">
+        <v>434</v>
+      </c>
+      <c r="C388" t="s">
+        <v>435</v>
+      </c>
+      <c r="D388" t="s">
+        <v>436</v>
+      </c>
+      <c r="E388" t="s">
+        <v>86</v>
+      </c>
+      <c r="F388" t="s">
+        <v>166</v>
+      </c>
+      <c r="G388" t="s">
+        <v>408</v>
+      </c>
+      <c r="H388">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B389" t="s">
+        <v>437</v>
+      </c>
+      <c r="C389" t="s">
+        <v>438</v>
+      </c>
+      <c r="D389" t="s">
+        <v>439</v>
+      </c>
+      <c r="E389" t="s">
+        <v>86</v>
+      </c>
+      <c r="F389" t="s">
+        <v>166</v>
+      </c>
+      <c r="G389" t="s">
+        <v>408</v>
+      </c>
+      <c r="H389">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B390" t="s">
+        <v>440</v>
+      </c>
+      <c r="C390" t="s">
+        <v>441</v>
+      </c>
+      <c r="D390" t="s">
+        <v>442</v>
+      </c>
+      <c r="E390" t="s">
+        <v>86</v>
+      </c>
+      <c r="F390" t="s">
+        <v>166</v>
+      </c>
+      <c r="G390" t="s">
+        <v>408</v>
+      </c>
+      <c r="H390">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B391" t="s">
+        <v>443</v>
+      </c>
+      <c r="C391" t="s">
+        <v>444</v>
+      </c>
+      <c r="D391" t="s">
+        <v>445</v>
+      </c>
+      <c r="E391" t="s">
+        <v>86</v>
+      </c>
+      <c r="F391" t="s">
+        <v>166</v>
+      </c>
+      <c r="G391" t="s">
+        <v>408</v>
+      </c>
+      <c r="H391">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B392" t="s">
+        <v>446</v>
+      </c>
+      <c r="C392" t="s">
+        <v>447</v>
+      </c>
+      <c r="D392" t="s">
+        <v>448</v>
+      </c>
+      <c r="E392" t="s">
+        <v>86</v>
+      </c>
+      <c r="F392" t="s">
+        <v>166</v>
+      </c>
+      <c r="G392" t="s">
+        <v>408</v>
+      </c>
+      <c r="H392">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B393" t="s">
+        <v>449</v>
+      </c>
+      <c r="C393" t="s">
+        <v>450</v>
+      </c>
+      <c r="D393" t="s">
+        <v>451</v>
+      </c>
+      <c r="E393" t="s">
+        <v>86</v>
+      </c>
+      <c r="F393" t="s">
+        <v>166</v>
+      </c>
+      <c r="G393" t="s">
+        <v>408</v>
+      </c>
+      <c r="H393">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B394" t="s">
+        <v>452</v>
+      </c>
+      <c r="C394" t="s">
+        <v>453</v>
+      </c>
+      <c r="D394" t="s">
+        <v>454</v>
+      </c>
+      <c r="E394" t="s">
+        <v>86</v>
+      </c>
+      <c r="F394" t="s">
+        <v>166</v>
+      </c>
+      <c r="G394" t="s">
+        <v>408</v>
+      </c>
+      <c r="H394">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B395" t="s">
+        <v>455</v>
+      </c>
+      <c r="C395" t="s">
+        <v>456</v>
+      </c>
+      <c r="D395" t="s">
+        <v>457</v>
+      </c>
+      <c r="E395" t="s">
+        <v>86</v>
+      </c>
+      <c r="F395" t="s">
+        <v>166</v>
+      </c>
+      <c r="G395" t="s">
+        <v>408</v>
+      </c>
+      <c r="H395">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B396" t="s">
+        <v>458</v>
+      </c>
+      <c r="C396" t="s">
+        <v>459</v>
+      </c>
+      <c r="D396" t="s">
+        <v>460</v>
+      </c>
+      <c r="E396" t="s">
+        <v>86</v>
+      </c>
+      <c r="F396" t="s">
+        <v>166</v>
+      </c>
+      <c r="G396" t="s">
+        <v>408</v>
+      </c>
+      <c r="H396">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B397" t="s">
+        <v>461</v>
+      </c>
+      <c r="C397" t="s">
+        <v>462</v>
+      </c>
+      <c r="D397" t="s">
+        <v>463</v>
+      </c>
+      <c r="E397" t="s">
+        <v>86</v>
+      </c>
+      <c r="F397" t="s">
+        <v>166</v>
+      </c>
+      <c r="G397" t="s">
+        <v>408</v>
+      </c>
+      <c r="H397">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B398" t="s">
+        <v>464</v>
+      </c>
+      <c r="C398" t="s">
+        <v>465</v>
+      </c>
+      <c r="D398" t="s">
+        <v>466</v>
+      </c>
+      <c r="E398" t="s">
+        <v>86</v>
+      </c>
+      <c r="F398" t="s">
+        <v>166</v>
+      </c>
+      <c r="G398" t="s">
+        <v>408</v>
+      </c>
+      <c r="H398">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B399" t="s">
+        <v>467</v>
+      </c>
+      <c r="C399" t="s">
+        <v>468</v>
+      </c>
+      <c r="D399" t="s">
+        <v>469</v>
+      </c>
+      <c r="E399" t="s">
+        <v>86</v>
+      </c>
+      <c r="F399" t="s">
+        <v>166</v>
+      </c>
+      <c r="G399" t="s">
+        <v>408</v>
+      </c>
+      <c r="H399">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B400" t="s">
+        <v>470</v>
+      </c>
+      <c r="C400" t="s">
+        <v>471</v>
+      </c>
+      <c r="D400" t="s">
+        <v>472</v>
+      </c>
+      <c r="E400" t="s">
+        <v>86</v>
+      </c>
+      <c r="F400" t="s">
+        <v>166</v>
+      </c>
+      <c r="G400" t="s">
+        <v>408</v>
+      </c>
+      <c r="H400">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B401" t="s">
+        <v>473</v>
+      </c>
+      <c r="C401" t="s">
+        <v>474</v>
+      </c>
+      <c r="D401" t="s">
+        <v>475</v>
+      </c>
+      <c r="E401" t="s">
+        <v>86</v>
+      </c>
+      <c r="F401" t="s">
+        <v>166</v>
+      </c>
+      <c r="G401" t="s">
+        <v>408</v>
+      </c>
+      <c r="H401">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B402" t="s">
+        <v>476</v>
+      </c>
+      <c r="C402" t="s">
+        <v>477</v>
+      </c>
+      <c r="D402" t="s">
+        <v>478</v>
+      </c>
+      <c r="E402" t="s">
+        <v>86</v>
+      </c>
+      <c r="F402" t="s">
+        <v>166</v>
+      </c>
+      <c r="G402" t="s">
+        <v>408</v>
+      </c>
+      <c r="H402">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B403" t="s">
+        <v>479</v>
+      </c>
+      <c r="C403" t="s">
+        <v>444</v>
+      </c>
+      <c r="D403" t="s">
+        <v>445</v>
+      </c>
+      <c r="E403" t="s">
+        <v>86</v>
+      </c>
+      <c r="F403" t="s">
+        <v>166</v>
+      </c>
+      <c r="G403" t="s">
+        <v>480</v>
+      </c>
+      <c r="H403">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B404" t="s">
+        <v>481</v>
+      </c>
+      <c r="C404" t="s">
+        <v>482</v>
+      </c>
+      <c r="D404" t="s">
+        <v>483</v>
+      </c>
+      <c r="E404" t="s">
+        <v>86</v>
+      </c>
+      <c r="F404" t="s">
+        <v>166</v>
+      </c>
+      <c r="G404" t="s">
+        <v>480</v>
+      </c>
+      <c r="H404">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B405" t="s">
+        <v>484</v>
+      </c>
+      <c r="C405" t="s">
+        <v>485</v>
+      </c>
+      <c r="D405" t="s">
+        <v>486</v>
+      </c>
+      <c r="E405" t="s">
+        <v>86</v>
+      </c>
+      <c r="F405" t="s">
+        <v>166</v>
+      </c>
+      <c r="G405" t="s">
+        <v>480</v>
+      </c>
+      <c r="H405">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B406" t="s">
+        <v>487</v>
+      </c>
+      <c r="C406" t="s">
+        <v>488</v>
+      </c>
+      <c r="D406" t="s">
+        <v>489</v>
+      </c>
+      <c r="E406" t="s">
+        <v>86</v>
+      </c>
+      <c r="F406" t="s">
+        <v>166</v>
+      </c>
+      <c r="G406" t="s">
+        <v>480</v>
+      </c>
+      <c r="H406">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B407" t="s">
+        <v>490</v>
+      </c>
+      <c r="C407" t="s">
+        <v>491</v>
+      </c>
+      <c r="D407" t="s">
+        <v>492</v>
+      </c>
+      <c r="E407" t="s">
+        <v>86</v>
+      </c>
+      <c r="F407" t="s">
+        <v>166</v>
+      </c>
+      <c r="G407" t="s">
+        <v>480</v>
+      </c>
+      <c r="H407">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B408" t="s">
+        <v>493</v>
+      </c>
+      <c r="C408" t="s">
+        <v>494</v>
+      </c>
+      <c r="D408" t="s">
+        <v>495</v>
+      </c>
+      <c r="E408" t="s">
+        <v>86</v>
+      </c>
+      <c r="F408" t="s">
+        <v>166</v>
+      </c>
+      <c r="G408" t="s">
+        <v>480</v>
+      </c>
+      <c r="H408">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B409" t="s">
+        <v>496</v>
+      </c>
+      <c r="C409" t="s">
+        <v>497</v>
+      </c>
+      <c r="D409" t="s">
+        <v>498</v>
+      </c>
+      <c r="E409" t="s">
+        <v>86</v>
+      </c>
+      <c r="F409" t="s">
+        <v>166</v>
+      </c>
+      <c r="G409" t="s">
+        <v>480</v>
+      </c>
+      <c r="H409">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B410" t="s">
+        <v>499</v>
+      </c>
+      <c r="C410" t="s">
+        <v>441</v>
+      </c>
+      <c r="D410" t="s">
+        <v>442</v>
+      </c>
+      <c r="E410" t="s">
+        <v>86</v>
+      </c>
+      <c r="F410" t="s">
+        <v>166</v>
+      </c>
+      <c r="G410" t="s">
+        <v>480</v>
+      </c>
+      <c r="H410">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B411" t="s">
+        <v>500</v>
+      </c>
+      <c r="C411" t="s">
+        <v>501</v>
+      </c>
+      <c r="D411" t="s">
+        <v>502</v>
+      </c>
+      <c r="E411" t="s">
+        <v>86</v>
+      </c>
+      <c r="F411" t="s">
+        <v>166</v>
+      </c>
+      <c r="G411" t="s">
+        <v>480</v>
+      </c>
+      <c r="H411">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B412" t="s">
+        <v>503</v>
+      </c>
+      <c r="C412" t="s">
+        <v>504</v>
+      </c>
+      <c r="D412" t="s">
+        <v>505</v>
+      </c>
+      <c r="E412" t="s">
+        <v>86</v>
+      </c>
+      <c r="F412" t="s">
+        <v>166</v>
+      </c>
+      <c r="G412" t="s">
+        <v>480</v>
+      </c>
+      <c r="H412">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B413" t="s">
+        <v>506</v>
+      </c>
+      <c r="C413" t="s">
+        <v>450</v>
+      </c>
+      <c r="D413" t="s">
+        <v>451</v>
+      </c>
+      <c r="E413" t="s">
+        <v>86</v>
+      </c>
+      <c r="F413" t="s">
+        <v>166</v>
+      </c>
+      <c r="G413" t="s">
+        <v>480</v>
+      </c>
+      <c r="H413">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B414" t="s">
+        <v>507</v>
+      </c>
+      <c r="C414" t="s">
+        <v>508</v>
+      </c>
+      <c r="D414" t="s">
+        <v>509</v>
+      </c>
+      <c r="E414" t="s">
+        <v>86</v>
+      </c>
+      <c r="F414" t="s">
+        <v>166</v>
+      </c>
+      <c r="G414" t="s">
+        <v>480</v>
+      </c>
+      <c r="H414">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B415" t="s">
+        <v>510</v>
+      </c>
+      <c r="C415" t="s">
+        <v>511</v>
+      </c>
+      <c r="D415" t="s">
+        <v>512</v>
+      </c>
+      <c r="E415" t="s">
+        <v>86</v>
+      </c>
+      <c r="F415" t="s">
+        <v>166</v>
+      </c>
+      <c r="G415" t="s">
+        <v>480</v>
+      </c>
+      <c r="H415">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B416" t="s">
+        <v>513</v>
+      </c>
+      <c r="C416" t="s">
+        <v>459</v>
+      </c>
+      <c r="D416" t="s">
+        <v>460</v>
+      </c>
+      <c r="E416" t="s">
+        <v>86</v>
+      </c>
+      <c r="F416" t="s">
+        <v>166</v>
+      </c>
+      <c r="G416" t="s">
+        <v>480</v>
+      </c>
+      <c r="H416">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B417" t="s">
+        <v>514</v>
+      </c>
+      <c r="C417" t="s">
+        <v>515</v>
+      </c>
+      <c r="D417" t="s">
+        <v>516</v>
+      </c>
+      <c r="E417" t="s">
+        <v>86</v>
+      </c>
+      <c r="F417" t="s">
+        <v>166</v>
+      </c>
+      <c r="G417" t="s">
+        <v>480</v>
+      </c>
+      <c r="H417">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B418" t="s">
+        <v>517</v>
+      </c>
+      <c r="C418" t="s">
+        <v>518</v>
+      </c>
+      <c r="D418" t="s">
+        <v>519</v>
+      </c>
+      <c r="E418" t="s">
+        <v>86</v>
+      </c>
+      <c r="F418" t="s">
+        <v>166</v>
+      </c>
+      <c r="G418" t="s">
+        <v>480</v>
+      </c>
+      <c r="H418">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B419" t="s">
+        <v>520</v>
+      </c>
+      <c r="C419" t="s">
+        <v>491</v>
+      </c>
+      <c r="D419" t="s">
+        <v>492</v>
+      </c>
+      <c r="E419" t="s">
+        <v>86</v>
+      </c>
+      <c r="F419" t="s">
+        <v>166</v>
+      </c>
+      <c r="G419" t="s">
+        <v>480</v>
+      </c>
+      <c r="H419">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B420" t="s">
+        <v>521</v>
+      </c>
+      <c r="C420" t="s">
+        <v>522</v>
+      </c>
+      <c r="D420" t="s">
+        <v>523</v>
+      </c>
+      <c r="E420" t="s">
+        <v>86</v>
+      </c>
+      <c r="F420" t="s">
+        <v>166</v>
+      </c>
+      <c r="G420" t="s">
+        <v>480</v>
+      </c>
+      <c r="H420">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B421" t="s">
+        <v>524</v>
+      </c>
+      <c r="C421" t="s">
+        <v>525</v>
+      </c>
+      <c r="D421" t="s">
+        <v>526</v>
+      </c>
+      <c r="E421" t="s">
+        <v>86</v>
+      </c>
+      <c r="F421" t="s">
+        <v>166</v>
+      </c>
+      <c r="G421" t="s">
+        <v>480</v>
+      </c>
+      <c r="H421">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B422" t="s">
+        <v>527</v>
+      </c>
+      <c r="C422" t="s">
+        <v>528</v>
+      </c>
+      <c r="D422" t="s">
+        <v>529</v>
+      </c>
+      <c r="E422" t="s">
+        <v>86</v>
+      </c>
+      <c r="F422" t="s">
+        <v>166</v>
+      </c>
+      <c r="G422" t="s">
+        <v>480</v>
+      </c>
+      <c r="H422">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B423" t="s">
+        <v>530</v>
+      </c>
+      <c r="C423" t="s">
+        <v>420</v>
+      </c>
+      <c r="D423" t="s">
+        <v>531</v>
+      </c>
+      <c r="E423" t="s">
+        <v>86</v>
+      </c>
+      <c r="F423" t="s">
+        <v>166</v>
+      </c>
+      <c r="G423" t="s">
+        <v>532</v>
+      </c>
+      <c r="H423">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B424" t="s">
+        <v>533</v>
+      </c>
+      <c r="C424" t="s">
+        <v>423</v>
+      </c>
+      <c r="D424" t="s">
+        <v>534</v>
+      </c>
+      <c r="E424" t="s">
+        <v>86</v>
+      </c>
+      <c r="F424" t="s">
+        <v>166</v>
+      </c>
+      <c r="G424" t="s">
+        <v>532</v>
+      </c>
+      <c r="H424">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B425" t="s">
+        <v>535</v>
+      </c>
+      <c r="C425" t="s">
+        <v>536</v>
+      </c>
+      <c r="D425" t="s">
+        <v>537</v>
+      </c>
+      <c r="E425" t="s">
+        <v>86</v>
+      </c>
+      <c r="F425" t="s">
+        <v>166</v>
+      </c>
+      <c r="G425" t="s">
+        <v>532</v>
+      </c>
+      <c r="H425">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B426" t="s">
+        <v>538</v>
+      </c>
+      <c r="C426" t="s">
+        <v>539</v>
+      </c>
+      <c r="D426" t="s">
+        <v>540</v>
+      </c>
+      <c r="E426" t="s">
+        <v>86</v>
+      </c>
+      <c r="F426" t="s">
+        <v>166</v>
+      </c>
+      <c r="G426" t="s">
+        <v>532</v>
+      </c>
+      <c r="H426">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B427" t="s">
+        <v>541</v>
+      </c>
+      <c r="C427" t="s">
+        <v>542</v>
+      </c>
+      <c r="D427" t="s">
+        <v>543</v>
+      </c>
+      <c r="E427" t="s">
+        <v>86</v>
+      </c>
+      <c r="F427" t="s">
+        <v>166</v>
+      </c>
+      <c r="G427" t="s">
+        <v>532</v>
+      </c>
+      <c r="H427">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B428" t="s">
+        <v>544</v>
+      </c>
+      <c r="C428" t="s">
+        <v>545</v>
+      </c>
+      <c r="D428" t="s">
+        <v>546</v>
+      </c>
+      <c r="E428" t="s">
+        <v>86</v>
+      </c>
+      <c r="F428" t="s">
+        <v>166</v>
+      </c>
+      <c r="G428" t="s">
+        <v>532</v>
+      </c>
+      <c r="H428">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B429" t="s">
+        <v>547</v>
+      </c>
+      <c r="C429" t="s">
+        <v>548</v>
+      </c>
+      <c r="D429" t="s">
+        <v>549</v>
+      </c>
+      <c r="E429" t="s">
+        <v>86</v>
+      </c>
+      <c r="F429" t="s">
+        <v>166</v>
+      </c>
+      <c r="G429" t="s">
+        <v>532</v>
+      </c>
+      <c r="H429">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B430" t="s">
+        <v>550</v>
+      </c>
+      <c r="C430" t="s">
+        <v>551</v>
+      </c>
+      <c r="D430" t="s">
+        <v>552</v>
+      </c>
+      <c r="E430" t="s">
+        <v>86</v>
+      </c>
+      <c r="F430" t="s">
+        <v>166</v>
+      </c>
+      <c r="G430" t="s">
+        <v>532</v>
+      </c>
+      <c r="H430">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B431" t="s">
+        <v>553</v>
+      </c>
+      <c r="C431" t="s">
+        <v>554</v>
+      </c>
+      <c r="D431" t="s">
+        <v>555</v>
+      </c>
+      <c r="E431" t="s">
+        <v>86</v>
+      </c>
+      <c r="F431" t="s">
+        <v>166</v>
+      </c>
+      <c r="G431" t="s">
+        <v>532</v>
+      </c>
+      <c r="H431">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B432" t="s">
+        <v>556</v>
+      </c>
+      <c r="C432" t="s">
+        <v>557</v>
+      </c>
+      <c r="D432" t="s">
+        <v>558</v>
+      </c>
+      <c r="E432" t="s">
+        <v>86</v>
+      </c>
+      <c r="F432" t="s">
+        <v>166</v>
+      </c>
+      <c r="G432" t="s">
+        <v>532</v>
+      </c>
+      <c r="H432">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B433" t="s">
+        <v>559</v>
+      </c>
+      <c r="C433" t="s">
+        <v>560</v>
+      </c>
+      <c r="D433" t="s">
+        <v>561</v>
+      </c>
+      <c r="E433" t="s">
+        <v>86</v>
+      </c>
+      <c r="F433" t="s">
+        <v>166</v>
+      </c>
+      <c r="G433" t="s">
+        <v>532</v>
+      </c>
+      <c r="H433">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B434" t="s">
+        <v>562</v>
+      </c>
+      <c r="C434" t="s">
+        <v>563</v>
+      </c>
+      <c r="D434" t="s">
+        <v>564</v>
+      </c>
+      <c r="E434" t="s">
+        <v>86</v>
+      </c>
+      <c r="F434" t="s">
+        <v>166</v>
+      </c>
+      <c r="G434" t="s">
+        <v>532</v>
+      </c>
+      <c r="H434">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B435" t="s">
+        <v>565</v>
+      </c>
+      <c r="C435" t="s">
+        <v>566</v>
+      </c>
+      <c r="D435" t="s">
+        <v>567</v>
+      </c>
+      <c r="E435" t="s">
+        <v>86</v>
+      </c>
+      <c r="F435" t="s">
+        <v>166</v>
+      </c>
+      <c r="G435" t="s">
+        <v>532</v>
+      </c>
+      <c r="H435">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B436" t="s">
+        <v>568</v>
+      </c>
+      <c r="C436" t="s">
+        <v>468</v>
+      </c>
+      <c r="D436" t="s">
+        <v>569</v>
+      </c>
+      <c r="E436" t="s">
+        <v>86</v>
+      </c>
+      <c r="F436" t="s">
+        <v>166</v>
+      </c>
+      <c r="G436" t="s">
+        <v>532</v>
+      </c>
+      <c r="H436">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B437" t="s">
+        <v>570</v>
+      </c>
+      <c r="C437" t="s">
+        <v>571</v>
+      </c>
+      <c r="D437" t="s">
+        <v>572</v>
+      </c>
+      <c r="E437" t="s">
+        <v>86</v>
+      </c>
+      <c r="F437" t="s">
+        <v>166</v>
+      </c>
+      <c r="G437" t="s">
+        <v>532</v>
+      </c>
+      <c r="H437">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B438" t="s">
+        <v>573</v>
+      </c>
+      <c r="C438" t="s">
+        <v>459</v>
+      </c>
+      <c r="D438" t="s">
+        <v>574</v>
+      </c>
+      <c r="E438" t="s">
+        <v>86</v>
+      </c>
+      <c r="F438" t="s">
+        <v>166</v>
+      </c>
+      <c r="G438" t="s">
+        <v>532</v>
+      </c>
+      <c r="H438">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B439" t="s">
+        <v>575</v>
+      </c>
+      <c r="C439" t="s">
+        <v>576</v>
+      </c>
+      <c r="D439" t="s">
+        <v>577</v>
+      </c>
+      <c r="E439" t="s">
+        <v>86</v>
+      </c>
+      <c r="F439" t="s">
+        <v>166</v>
+      </c>
+      <c r="G439" t="s">
+        <v>532</v>
+      </c>
+      <c r="H439">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B440" t="s">
+        <v>578</v>
+      </c>
+      <c r="C440" t="s">
+        <v>579</v>
+      </c>
+      <c r="D440" t="s">
+        <v>580</v>
+      </c>
+      <c r="E440" t="s">
+        <v>86</v>
+      </c>
+      <c r="F440" t="s">
+        <v>166</v>
+      </c>
+      <c r="G440" t="s">
+        <v>532</v>
+      </c>
+      <c r="H440">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B441" t="s">
+        <v>581</v>
+      </c>
+      <c r="C441" t="s">
+        <v>582</v>
+      </c>
+      <c r="D441" t="s">
+        <v>583</v>
+      </c>
+      <c r="E441" t="s">
+        <v>86</v>
+      </c>
+      <c r="F441" t="s">
+        <v>166</v>
+      </c>
+      <c r="G441" t="s">
+        <v>532</v>
+      </c>
+      <c r="H441">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B442" t="s">
+        <v>584</v>
+      </c>
+      <c r="C442" t="s">
+        <v>585</v>
+      </c>
+      <c r="D442" t="s">
+        <v>586</v>
+      </c>
+      <c r="E442" t="s">
+        <v>86</v>
+      </c>
+      <c r="F442" t="s">
+        <v>166</v>
+      </c>
+      <c r="G442" t="s">
+        <v>532</v>
+      </c>
+      <c r="H442">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B443" t="s">
+        <v>587</v>
+      </c>
+      <c r="C443" t="s">
+        <v>420</v>
+      </c>
+      <c r="D443" t="s">
+        <v>421</v>
+      </c>
+      <c r="E443" t="s">
+        <v>86</v>
+      </c>
+      <c r="F443" t="s">
+        <v>166</v>
+      </c>
+      <c r="G443" t="s">
+        <v>588</v>
+      </c>
+      <c r="H443">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B444" t="s">
+        <v>589</v>
+      </c>
+      <c r="C444" t="s">
+        <v>423</v>
+      </c>
+      <c r="D444" t="s">
+        <v>424</v>
+      </c>
+      <c r="E444" t="s">
+        <v>86</v>
+      </c>
+      <c r="F444" t="s">
+        <v>166</v>
+      </c>
+      <c r="G444" t="s">
+        <v>588</v>
+      </c>
+      <c r="H444">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B445" t="s">
+        <v>590</v>
+      </c>
+      <c r="C445" t="s">
+        <v>536</v>
+      </c>
+      <c r="D445" t="s">
+        <v>591</v>
+      </c>
+      <c r="E445" t="s">
+        <v>86</v>
+      </c>
+      <c r="F445" t="s">
+        <v>166</v>
+      </c>
+      <c r="G445" t="s">
+        <v>588</v>
+      </c>
+      <c r="H445">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B446" t="s">
+        <v>592</v>
+      </c>
+      <c r="C446" t="s">
+        <v>539</v>
+      </c>
+      <c r="D446" t="s">
+        <v>593</v>
+      </c>
+      <c r="E446" t="s">
+        <v>86</v>
+      </c>
+      <c r="F446" t="s">
+        <v>166</v>
+      </c>
+      <c r="G446" t="s">
+        <v>588</v>
+      </c>
+      <c r="H446">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B447" t="s">
+        <v>594</v>
+      </c>
+      <c r="C447" t="s">
+        <v>542</v>
+      </c>
+      <c r="D447" t="s">
+        <v>595</v>
+      </c>
+      <c r="E447" t="s">
+        <v>86</v>
+      </c>
+      <c r="F447" t="s">
+        <v>166</v>
+      </c>
+      <c r="G447" t="s">
+        <v>588</v>
+      </c>
+      <c r="H447">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B448" t="s">
+        <v>596</v>
+      </c>
+      <c r="C448" t="s">
+        <v>545</v>
+      </c>
+      <c r="D448" t="s">
+        <v>597</v>
+      </c>
+      <c r="E448" t="s">
+        <v>86</v>
+      </c>
+      <c r="F448" t="s">
+        <v>166</v>
+      </c>
+      <c r="G448" t="s">
+        <v>588</v>
+      </c>
+      <c r="H448">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B449" t="s">
+        <v>598</v>
+      </c>
+      <c r="C449" t="s">
+        <v>548</v>
+      </c>
+      <c r="D449" t="s">
+        <v>599</v>
+      </c>
+      <c r="E449" t="s">
+        <v>86</v>
+      </c>
+      <c r="F449" t="s">
+        <v>166</v>
+      </c>
+      <c r="G449" t="s">
+        <v>588</v>
+      </c>
+      <c r="H449">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B450" t="s">
+        <v>600</v>
+      </c>
+      <c r="C450" t="s">
+        <v>551</v>
+      </c>
+      <c r="D450" t="s">
+        <v>601</v>
+      </c>
+      <c r="E450" t="s">
+        <v>86</v>
+      </c>
+      <c r="F450" t="s">
+        <v>166</v>
+      </c>
+      <c r="G450" t="s">
+        <v>588</v>
+      </c>
+      <c r="H450">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B451" t="s">
+        <v>602</v>
+      </c>
+      <c r="C451" t="s">
+        <v>554</v>
+      </c>
+      <c r="D451" t="s">
+        <v>603</v>
+      </c>
+      <c r="E451" t="s">
+        <v>86</v>
+      </c>
+      <c r="F451" t="s">
+        <v>166</v>
+      </c>
+      <c r="G451" t="s">
+        <v>588</v>
+      </c>
+      <c r="H451">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="452" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B452" t="s">
+        <v>604</v>
+      </c>
+      <c r="C452" t="s">
+        <v>557</v>
+      </c>
+      <c r="D452" t="s">
+        <v>605</v>
+      </c>
+      <c r="E452" t="s">
+        <v>86</v>
+      </c>
+      <c r="F452" t="s">
+        <v>166</v>
+      </c>
+      <c r="G452" t="s">
+        <v>588</v>
+      </c>
+      <c r="H452">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B453" t="s">
+        <v>606</v>
+      </c>
+      <c r="C453" t="s">
+        <v>560</v>
+      </c>
+      <c r="D453" t="s">
+        <v>607</v>
+      </c>
+      <c r="E453" t="s">
+        <v>86</v>
+      </c>
+      <c r="F453" t="s">
+        <v>166</v>
+      </c>
+      <c r="G453" t="s">
+        <v>588</v>
+      </c>
+      <c r="H453">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B454" t="s">
+        <v>608</v>
+      </c>
+      <c r="C454" t="s">
+        <v>563</v>
+      </c>
+      <c r="D454" t="s">
+        <v>609</v>
+      </c>
+      <c r="E454" t="s">
+        <v>86</v>
+      </c>
+      <c r="F454" t="s">
+        <v>166</v>
+      </c>
+      <c r="G454" t="s">
+        <v>588</v>
+      </c>
+      <c r="H454">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="455" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B455" t="s">
+        <v>610</v>
+      </c>
+      <c r="C455" t="s">
+        <v>566</v>
+      </c>
+      <c r="D455" t="s">
+        <v>611</v>
+      </c>
+      <c r="E455" t="s">
+        <v>86</v>
+      </c>
+      <c r="F455" t="s">
+        <v>166</v>
+      </c>
+      <c r="G455" t="s">
+        <v>588</v>
+      </c>
+      <c r="H455">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B456" t="s">
+        <v>612</v>
+      </c>
+      <c r="C456" t="s">
+        <v>468</v>
+      </c>
+      <c r="D456" t="s">
+        <v>469</v>
+      </c>
+      <c r="E456" t="s">
+        <v>86</v>
+      </c>
+      <c r="F456" t="s">
+        <v>166</v>
+      </c>
+      <c r="G456" t="s">
+        <v>588</v>
+      </c>
+      <c r="H456">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="457" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B457" t="s">
+        <v>613</v>
+      </c>
+      <c r="C457" t="s">
+        <v>571</v>
+      </c>
+      <c r="D457" t="s">
+        <v>614</v>
+      </c>
+      <c r="E457" t="s">
+        <v>86</v>
+      </c>
+      <c r="F457" t="s">
+        <v>166</v>
+      </c>
+      <c r="G457" t="s">
+        <v>588</v>
+      </c>
+      <c r="H457">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B458" t="s">
+        <v>615</v>
+      </c>
+      <c r="C458" t="s">
+        <v>459</v>
+      </c>
+      <c r="D458" t="s">
+        <v>460</v>
+      </c>
+      <c r="E458" t="s">
+        <v>86</v>
+      </c>
+      <c r="F458" t="s">
+        <v>166</v>
+      </c>
+      <c r="G458" t="s">
+        <v>588</v>
+      </c>
+      <c r="H458">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B459" t="s">
+        <v>616</v>
+      </c>
+      <c r="C459" t="s">
+        <v>576</v>
+      </c>
+      <c r="D459" t="s">
+        <v>617</v>
+      </c>
+      <c r="E459" t="s">
+        <v>86</v>
+      </c>
+      <c r="F459" t="s">
+        <v>166</v>
+      </c>
+      <c r="G459" t="s">
+        <v>588</v>
+      </c>
+      <c r="H459">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B460" t="s">
+        <v>618</v>
+      </c>
+      <c r="C460" t="s">
+        <v>579</v>
+      </c>
+      <c r="D460" t="s">
+        <v>619</v>
+      </c>
+      <c r="E460" t="s">
+        <v>86</v>
+      </c>
+      <c r="F460" t="s">
+        <v>166</v>
+      </c>
+      <c r="G460" t="s">
+        <v>588</v>
+      </c>
+      <c r="H460">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B461" t="s">
+        <v>620</v>
+      </c>
+      <c r="C461" t="s">
+        <v>582</v>
+      </c>
+      <c r="D461" t="s">
+        <v>621</v>
+      </c>
+      <c r="E461" t="s">
+        <v>86</v>
+      </c>
+      <c r="F461" t="s">
+        <v>166</v>
+      </c>
+      <c r="G461" t="s">
+        <v>588</v>
+      </c>
+      <c r="H461">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="462" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B462" t="s">
+        <v>622</v>
+      </c>
+      <c r="C462" t="s">
+        <v>585</v>
+      </c>
+      <c r="D462" t="s">
+        <v>623</v>
+      </c>
+      <c r="E462" t="s">
+        <v>86</v>
+      </c>
+      <c r="F462" t="s">
+        <v>166</v>
+      </c>
+      <c r="G462" t="s">
+        <v>588</v>
+      </c>
+      <c r="H462">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B463" t="s">
+        <v>624</v>
+      </c>
+      <c r="C463" t="s">
+        <v>420</v>
+      </c>
+      <c r="D463" t="s">
+        <v>421</v>
+      </c>
+      <c r="E463" t="s">
+        <v>86</v>
+      </c>
+      <c r="F463" t="s">
+        <v>166</v>
+      </c>
+      <c r="G463" t="s">
+        <v>625</v>
+      </c>
+      <c r="H463">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="464" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B464" t="s">
+        <v>626</v>
+      </c>
+      <c r="C464" t="s">
+        <v>423</v>
+      </c>
+      <c r="D464" t="s">
+        <v>424</v>
+      </c>
+      <c r="E464" t="s">
+        <v>86</v>
+      </c>
+      <c r="F464" t="s">
+        <v>166</v>
+      </c>
+      <c r="G464" t="s">
+        <v>625</v>
+      </c>
+      <c r="H464">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B465" t="s">
+        <v>627</v>
+      </c>
+      <c r="C465" t="s">
+        <v>536</v>
+      </c>
+      <c r="D465" t="s">
+        <v>591</v>
+      </c>
+      <c r="E465" t="s">
+        <v>86</v>
+      </c>
+      <c r="F465" t="s">
+        <v>166</v>
+      </c>
+      <c r="G465" t="s">
+        <v>625</v>
+      </c>
+      <c r="H465">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B466" t="s">
+        <v>628</v>
+      </c>
+      <c r="C466" t="s">
+        <v>539</v>
+      </c>
+      <c r="D466" t="s">
+        <v>593</v>
+      </c>
+      <c r="E466" t="s">
+        <v>86</v>
+      </c>
+      <c r="F466" t="s">
+        <v>166</v>
+      </c>
+      <c r="G466" t="s">
+        <v>625</v>
+      </c>
+      <c r="H466">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B467" t="s">
+        <v>629</v>
+      </c>
+      <c r="C467" t="s">
+        <v>542</v>
+      </c>
+      <c r="D467" t="s">
+        <v>595</v>
+      </c>
+      <c r="E467" t="s">
+        <v>86</v>
+      </c>
+      <c r="F467" t="s">
+        <v>166</v>
+      </c>
+      <c r="G467" t="s">
+        <v>625</v>
+      </c>
+      <c r="H467">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B468" t="s">
+        <v>630</v>
+      </c>
+      <c r="C468" t="s">
+        <v>545</v>
+      </c>
+      <c r="D468" t="s">
+        <v>597</v>
+      </c>
+      <c r="E468" t="s">
+        <v>86</v>
+      </c>
+      <c r="F468" t="s">
+        <v>166</v>
+      </c>
+      <c r="G468" t="s">
+        <v>625</v>
+      </c>
+      <c r="H468">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B469" t="s">
+        <v>631</v>
+      </c>
+      <c r="C469" t="s">
+        <v>548</v>
+      </c>
+      <c r="D469" t="s">
+        <v>599</v>
+      </c>
+      <c r="E469" t="s">
+        <v>86</v>
+      </c>
+      <c r="F469" t="s">
+        <v>166</v>
+      </c>
+      <c r="G469" t="s">
+        <v>625</v>
+      </c>
+      <c r="H469">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B470" t="s">
+        <v>632</v>
+      </c>
+      <c r="C470" t="s">
+        <v>551</v>
+      </c>
+      <c r="D470" t="s">
+        <v>601</v>
+      </c>
+      <c r="E470" t="s">
+        <v>86</v>
+      </c>
+      <c r="F470" t="s">
+        <v>166</v>
+      </c>
+      <c r="G470" t="s">
+        <v>625</v>
+      </c>
+      <c r="H470">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B471" t="s">
+        <v>633</v>
+      </c>
+      <c r="C471" t="s">
+        <v>554</v>
+      </c>
+      <c r="D471" t="s">
+        <v>603</v>
+      </c>
+      <c r="E471" t="s">
+        <v>86</v>
+      </c>
+      <c r="F471" t="s">
+        <v>166</v>
+      </c>
+      <c r="G471" t="s">
+        <v>625</v>
+      </c>
+      <c r="H471">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B472" t="s">
+        <v>634</v>
+      </c>
+      <c r="C472" t="s">
+        <v>557</v>
+      </c>
+      <c r="D472" t="s">
+        <v>605</v>
+      </c>
+      <c r="E472" t="s">
+        <v>86</v>
+      </c>
+      <c r="F472" t="s">
+        <v>166</v>
+      </c>
+      <c r="G472" t="s">
+        <v>625</v>
+      </c>
+      <c r="H472">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B473" t="s">
+        <v>635</v>
+      </c>
+      <c r="C473" t="s">
+        <v>560</v>
+      </c>
+      <c r="D473" t="s">
+        <v>607</v>
+      </c>
+      <c r="E473" t="s">
+        <v>86</v>
+      </c>
+      <c r="F473" t="s">
+        <v>166</v>
+      </c>
+      <c r="G473" t="s">
+        <v>625</v>
+      </c>
+      <c r="H473">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B474" t="s">
+        <v>636</v>
+      </c>
+      <c r="C474" t="s">
+        <v>563</v>
+      </c>
+      <c r="D474" t="s">
+        <v>609</v>
+      </c>
+      <c r="E474" t="s">
+        <v>86</v>
+      </c>
+      <c r="F474" t="s">
+        <v>166</v>
+      </c>
+      <c r="G474" t="s">
+        <v>625</v>
+      </c>
+      <c r="H474">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B475" t="s">
+        <v>637</v>
+      </c>
+      <c r="C475" t="s">
+        <v>566</v>
+      </c>
+      <c r="D475" t="s">
+        <v>611</v>
+      </c>
+      <c r="E475" t="s">
+        <v>86</v>
+      </c>
+      <c r="F475" t="s">
+        <v>166</v>
+      </c>
+      <c r="G475" t="s">
+        <v>625</v>
+      </c>
+      <c r="H475">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B476" t="s">
+        <v>638</v>
+      </c>
+      <c r="C476" t="s">
+        <v>468</v>
+      </c>
+      <c r="D476" t="s">
+        <v>469</v>
+      </c>
+      <c r="E476" t="s">
+        <v>86</v>
+      </c>
+      <c r="F476" t="s">
+        <v>166</v>
+      </c>
+      <c r="G476" t="s">
+        <v>625</v>
+      </c>
+      <c r="H476">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B477" t="s">
+        <v>639</v>
+      </c>
+      <c r="C477" t="s">
+        <v>571</v>
+      </c>
+      <c r="D477" t="s">
+        <v>614</v>
+      </c>
+      <c r="E477" t="s">
+        <v>86</v>
+      </c>
+      <c r="F477" t="s">
+        <v>166</v>
+      </c>
+      <c r="G477" t="s">
+        <v>625</v>
+      </c>
+      <c r="H477">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B478" t="s">
+        <v>640</v>
+      </c>
+      <c r="C478" t="s">
+        <v>459</v>
+      </c>
+      <c r="D478" t="s">
+        <v>460</v>
+      </c>
+      <c r="E478" t="s">
+        <v>86</v>
+      </c>
+      <c r="F478" t="s">
+        <v>166</v>
+      </c>
+      <c r="G478" t="s">
+        <v>625</v>
+      </c>
+      <c r="H478">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B479" t="s">
+        <v>641</v>
+      </c>
+      <c r="C479" t="s">
+        <v>576</v>
+      </c>
+      <c r="D479" t="s">
+        <v>617</v>
+      </c>
+      <c r="E479" t="s">
+        <v>86</v>
+      </c>
+      <c r="F479" t="s">
+        <v>166</v>
+      </c>
+      <c r="G479" t="s">
+        <v>625</v>
+      </c>
+      <c r="H479">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B480" t="s">
+        <v>642</v>
+      </c>
+      <c r="C480" t="s">
+        <v>579</v>
+      </c>
+      <c r="D480" t="s">
+        <v>619</v>
+      </c>
+      <c r="E480" t="s">
+        <v>86</v>
+      </c>
+      <c r="F480" t="s">
+        <v>166</v>
+      </c>
+      <c r="G480" t="s">
+        <v>625</v>
+      </c>
+      <c r="H480">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B481" t="s">
+        <v>643</v>
+      </c>
+      <c r="C481" t="s">
+        <v>582</v>
+      </c>
+      <c r="D481" t="s">
+        <v>621</v>
+      </c>
+      <c r="E481" t="s">
+        <v>86</v>
+      </c>
+      <c r="F481" t="s">
+        <v>166</v>
+      </c>
+      <c r="G481" t="s">
+        <v>625</v>
+      </c>
+      <c r="H481">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B482" t="s">
+        <v>644</v>
+      </c>
+      <c r="C482" t="s">
+        <v>585</v>
+      </c>
+      <c r="D482" t="s">
+        <v>623</v>
+      </c>
+      <c r="E482" t="s">
+        <v>86</v>
+      </c>
+      <c r="F482" t="s">
+        <v>166</v>
+      </c>
+      <c r="G482" t="s">
+        <v>625</v>
+      </c>
+      <c r="H482">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B483" t="s">
+        <v>645</v>
+      </c>
+      <c r="C483" t="s">
+        <v>646</v>
+      </c>
+      <c r="D483" t="s">
+        <v>647</v>
+      </c>
+      <c r="E483" t="s">
+        <v>86</v>
+      </c>
+      <c r="F483" t="s">
+        <v>166</v>
+      </c>
+      <c r="G483" t="s">
+        <v>648</v>
+      </c>
+      <c r="H483">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B484" t="s">
+        <v>481</v>
+      </c>
+      <c r="C484" t="s">
+        <v>649</v>
+      </c>
+      <c r="D484" t="s">
+        <v>650</v>
+      </c>
+      <c r="E484" t="s">
+        <v>86</v>
+      </c>
+      <c r="F484" t="s">
+        <v>166</v>
+      </c>
+      <c r="G484" t="s">
+        <v>648</v>
+      </c>
+      <c r="H484">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B485" t="s">
+        <v>651</v>
+      </c>
+      <c r="C485" t="s">
+        <v>536</v>
+      </c>
+      <c r="D485" t="s">
+        <v>652</v>
+      </c>
+      <c r="E485" t="s">
+        <v>86</v>
+      </c>
+      <c r="F485" t="s">
+        <v>166</v>
+      </c>
+      <c r="G485" t="s">
+        <v>648</v>
+      </c>
+      <c r="H485">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B486" t="s">
+        <v>653</v>
+      </c>
+      <c r="C486" t="s">
+        <v>654</v>
+      </c>
+      <c r="D486" t="s">
+        <v>655</v>
+      </c>
+      <c r="E486" t="s">
+        <v>86</v>
+      </c>
+      <c r="F486" t="s">
+        <v>166</v>
+      </c>
+      <c r="G486" t="s">
+        <v>648</v>
+      </c>
+      <c r="H486">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B487" t="s">
+        <v>656</v>
+      </c>
+      <c r="C487" t="s">
+        <v>542</v>
+      </c>
+      <c r="D487" t="s">
+        <v>543</v>
+      </c>
+      <c r="E487" t="s">
+        <v>86</v>
+      </c>
+      <c r="F487" t="s">
+        <v>166</v>
+      </c>
+      <c r="G487" t="s">
+        <v>648</v>
+      </c>
+      <c r="H487">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B488" t="s">
+        <v>657</v>
+      </c>
+      <c r="C488" t="s">
+        <v>658</v>
+      </c>
+      <c r="D488" t="s">
+        <v>659</v>
+      </c>
+      <c r="E488" t="s">
+        <v>86</v>
+      </c>
+      <c r="F488" t="s">
+        <v>166</v>
+      </c>
+      <c r="G488" t="s">
+        <v>648</v>
+      </c>
+      <c r="H488">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B489" t="s">
+        <v>660</v>
+      </c>
+      <c r="C489" t="s">
+        <v>661</v>
+      </c>
+      <c r="D489" t="s">
+        <v>549</v>
+      </c>
+      <c r="E489" t="s">
+        <v>86</v>
+      </c>
+      <c r="F489" t="s">
+        <v>166</v>
+      </c>
+      <c r="G489" t="s">
+        <v>648</v>
+      </c>
+      <c r="H489">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B490" t="s">
+        <v>662</v>
+      </c>
+      <c r="C490" t="s">
+        <v>663</v>
+      </c>
+      <c r="D490" t="s">
+        <v>664</v>
+      </c>
+      <c r="E490" t="s">
+        <v>86</v>
+      </c>
+      <c r="F490" t="s">
+        <v>166</v>
+      </c>
+      <c r="G490" t="s">
+        <v>648</v>
+      </c>
+      <c r="H490">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B491" t="s">
+        <v>665</v>
+      </c>
+      <c r="C491" t="s">
+        <v>554</v>
+      </c>
+      <c r="D491" t="s">
+        <v>555</v>
+      </c>
+      <c r="E491" t="s">
+        <v>86</v>
+      </c>
+      <c r="F491" t="s">
+        <v>166</v>
+      </c>
+      <c r="G491" t="s">
+        <v>648</v>
+      </c>
+      <c r="H491">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B492" t="s">
+        <v>666</v>
+      </c>
+      <c r="C492" t="s">
+        <v>557</v>
+      </c>
+      <c r="D492" t="s">
+        <v>558</v>
+      </c>
+      <c r="E492" t="s">
+        <v>86</v>
+      </c>
+      <c r="F492" t="s">
+        <v>166</v>
+      </c>
+      <c r="G492" t="s">
+        <v>648</v>
+      </c>
+      <c r="H492">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B493" t="s">
+        <v>667</v>
+      </c>
+      <c r="C493" t="s">
+        <v>668</v>
+      </c>
+      <c r="D493" t="s">
+        <v>669</v>
+      </c>
+      <c r="E493" t="s">
+        <v>86</v>
+      </c>
+      <c r="F493" t="s">
+        <v>166</v>
+      </c>
+      <c r="G493" t="s">
+        <v>648</v>
+      </c>
+      <c r="H493">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B494" t="s">
+        <v>670</v>
+      </c>
+      <c r="C494" t="s">
+        <v>563</v>
+      </c>
+      <c r="D494" t="s">
+        <v>671</v>
+      </c>
+      <c r="E494" t="s">
+        <v>86</v>
+      </c>
+      <c r="F494" t="s">
+        <v>166</v>
+      </c>
+      <c r="G494" t="s">
+        <v>648</v>
+      </c>
+      <c r="H494">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B495" t="s">
+        <v>672</v>
+      </c>
+      <c r="C495" t="s">
+        <v>485</v>
+      </c>
+      <c r="D495" t="s">
+        <v>673</v>
+      </c>
+      <c r="E495" t="s">
+        <v>86</v>
+      </c>
+      <c r="F495" t="s">
+        <v>166</v>
+      </c>
+      <c r="G495" t="s">
+        <v>648</v>
+      </c>
+      <c r="H495">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B496" t="s">
+        <v>674</v>
+      </c>
+      <c r="C496" t="s">
+        <v>435</v>
+      </c>
+      <c r="D496" t="s">
+        <v>569</v>
+      </c>
+      <c r="E496" t="s">
+        <v>86</v>
+      </c>
+      <c r="F496" t="s">
+        <v>166</v>
+      </c>
+      <c r="G496" t="s">
+        <v>648</v>
+      </c>
+      <c r="H496">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B497" t="s">
+        <v>479</v>
+      </c>
+      <c r="C497" t="s">
+        <v>444</v>
+      </c>
+      <c r="D497" t="s">
+        <v>675</v>
+      </c>
+      <c r="E497" t="s">
+        <v>86</v>
+      </c>
+      <c r="F497" t="s">
+        <v>166</v>
+      </c>
+      <c r="G497" t="s">
+        <v>648</v>
+      </c>
+      <c r="H497">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B498" t="s">
+        <v>676</v>
+      </c>
+      <c r="C498" t="s">
+        <v>677</v>
+      </c>
+      <c r="D498" t="s">
+        <v>678</v>
+      </c>
+      <c r="E498" t="s">
+        <v>86</v>
+      </c>
+      <c r="F498" t="s">
+        <v>166</v>
+      </c>
+      <c r="G498" t="s">
+        <v>648</v>
+      </c>
+      <c r="H498">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B499" t="s">
+        <v>679</v>
+      </c>
+      <c r="C499" t="s">
+        <v>576</v>
+      </c>
+      <c r="D499" t="s">
+        <v>577</v>
+      </c>
+      <c r="E499" t="s">
+        <v>86</v>
+      </c>
+      <c r="F499" t="s">
+        <v>166</v>
+      </c>
+      <c r="G499" t="s">
+        <v>648</v>
+      </c>
+      <c r="H499">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B500" t="s">
+        <v>680</v>
+      </c>
+      <c r="C500" t="s">
+        <v>579</v>
+      </c>
+      <c r="D500" t="s">
+        <v>681</v>
+      </c>
+      <c r="E500" t="s">
+        <v>86</v>
+      </c>
+      <c r="F500" t="s">
+        <v>166</v>
+      </c>
+      <c r="G500" t="s">
+        <v>648</v>
+      </c>
+      <c r="H500">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B501" t="s">
+        <v>682</v>
+      </c>
+      <c r="C501" t="s">
+        <v>582</v>
+      </c>
+      <c r="D501" t="s">
+        <v>583</v>
+      </c>
+      <c r="E501" t="s">
+        <v>86</v>
+      </c>
+      <c r="F501" t="s">
+        <v>166</v>
+      </c>
+      <c r="G501" t="s">
+        <v>648</v>
+      </c>
+      <c r="H501">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B502" t="s">
+        <v>683</v>
+      </c>
+      <c r="C502" t="s">
+        <v>684</v>
+      </c>
+      <c r="D502" t="s">
+        <v>685</v>
+      </c>
+      <c r="E502" t="s">
+        <v>86</v>
+      </c>
+      <c r="F502" t="s">
+        <v>166</v>
+      </c>
+      <c r="G502" t="s">
+        <v>648</v>
+      </c>
+      <c r="H502">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B503" t="s">
+        <v>686</v>
+      </c>
+      <c r="C503" t="s">
+        <v>687</v>
+      </c>
+      <c r="D503" t="s">
+        <v>688</v>
+      </c>
+      <c r="E503" t="s">
+        <v>86</v>
+      </c>
+      <c r="F503" t="s">
+        <v>166</v>
+      </c>
+      <c r="G503" t="s">
+        <v>689</v>
+      </c>
+      <c r="H503">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B504" t="s">
+        <v>690</v>
+      </c>
+      <c r="C504" t="s">
+        <v>691</v>
+      </c>
+      <c r="D504" t="s">
+        <v>692</v>
+      </c>
+      <c r="E504" t="s">
+        <v>86</v>
+      </c>
+      <c r="F504" t="s">
+        <v>166</v>
+      </c>
+      <c r="G504" t="s">
+        <v>689</v>
+      </c>
+      <c r="H504">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B505" t="s">
+        <v>693</v>
+      </c>
+      <c r="C505" t="s">
+        <v>694</v>
+      </c>
+      <c r="D505" t="s">
+        <v>695</v>
+      </c>
+      <c r="E505" t="s">
+        <v>86</v>
+      </c>
+      <c r="F505" t="s">
+        <v>166</v>
+      </c>
+      <c r="G505" t="s">
+        <v>689</v>
+      </c>
+      <c r="H505">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B506" t="s">
+        <v>696</v>
+      </c>
+      <c r="C506" t="s">
+        <v>697</v>
+      </c>
+      <c r="D506" t="s">
+        <v>698</v>
+      </c>
+      <c r="E506" t="s">
+        <v>86</v>
+      </c>
+      <c r="F506" t="s">
+        <v>166</v>
+      </c>
+      <c r="G506" t="s">
+        <v>689</v>
+      </c>
+      <c r="H506">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B507" t="s">
+        <v>699</v>
+      </c>
+      <c r="C507" t="s">
+        <v>435</v>
+      </c>
+      <c r="D507" t="s">
+        <v>700</v>
+      </c>
+      <c r="E507" t="s">
+        <v>86</v>
+      </c>
+      <c r="F507" t="s">
+        <v>166</v>
+      </c>
+      <c r="G507" t="s">
+        <v>689</v>
+      </c>
+      <c r="H507">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B508" t="s">
+        <v>701</v>
+      </c>
+      <c r="C508" t="s">
+        <v>702</v>
+      </c>
+      <c r="D508" t="s">
+        <v>703</v>
+      </c>
+      <c r="E508" t="s">
+        <v>86</v>
+      </c>
+      <c r="F508" t="s">
+        <v>166</v>
+      </c>
+      <c r="G508" t="s">
+        <v>689</v>
+      </c>
+      <c r="H508">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B509" t="s">
+        <v>704</v>
+      </c>
+      <c r="C509" t="s">
+        <v>661</v>
+      </c>
+      <c r="D509" t="s">
+        <v>705</v>
+      </c>
+      <c r="E509" t="s">
+        <v>86</v>
+      </c>
+      <c r="F509" t="s">
+        <v>166</v>
+      </c>
+      <c r="G509" t="s">
+        <v>689</v>
+      </c>
+      <c r="H509">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B510" t="s">
+        <v>706</v>
+      </c>
+      <c r="C510" t="s">
+        <v>663</v>
+      </c>
+      <c r="D510" t="s">
+        <v>707</v>
+      </c>
+      <c r="E510" t="s">
+        <v>86</v>
+      </c>
+      <c r="F510" t="s">
+        <v>166</v>
+      </c>
+      <c r="G510" t="s">
+        <v>689</v>
+      </c>
+      <c r="H510">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B511" t="s">
+        <v>708</v>
+      </c>
+      <c r="C511" t="s">
+        <v>709</v>
+      </c>
+      <c r="D511" t="s">
+        <v>710</v>
+      </c>
+      <c r="E511" t="s">
+        <v>86</v>
+      </c>
+      <c r="F511" t="s">
+        <v>166</v>
+      </c>
+      <c r="G511" t="s">
+        <v>689</v>
+      </c>
+      <c r="H511">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B512" t="s">
+        <v>711</v>
+      </c>
+      <c r="C512" t="s">
+        <v>557</v>
+      </c>
+      <c r="D512" t="s">
+        <v>712</v>
+      </c>
+      <c r="E512" t="s">
+        <v>86</v>
+      </c>
+      <c r="F512" t="s">
+        <v>166</v>
+      </c>
+      <c r="G512" t="s">
+        <v>689</v>
+      </c>
+      <c r="H512">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B513" t="s">
+        <v>713</v>
+      </c>
+      <c r="C513" t="s">
+        <v>714</v>
+      </c>
+      <c r="D513" t="s">
+        <v>715</v>
+      </c>
+      <c r="E513" t="s">
+        <v>86</v>
+      </c>
+      <c r="F513" t="s">
+        <v>166</v>
+      </c>
+      <c r="G513" t="s">
+        <v>689</v>
+      </c>
+      <c r="H513">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B514" t="s">
+        <v>716</v>
+      </c>
+      <c r="C514" t="s">
+        <v>563</v>
+      </c>
+      <c r="D514" t="s">
+        <v>717</v>
+      </c>
+      <c r="E514" t="s">
+        <v>86</v>
+      </c>
+      <c r="F514" t="s">
+        <v>166</v>
+      </c>
+      <c r="G514" t="s">
+        <v>689</v>
+      </c>
+      <c r="H514">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B515" t="s">
+        <v>718</v>
+      </c>
+      <c r="C515" t="s">
+        <v>719</v>
+      </c>
+      <c r="D515" t="s">
+        <v>720</v>
+      </c>
+      <c r="E515" t="s">
+        <v>86</v>
+      </c>
+      <c r="F515" t="s">
+        <v>166</v>
+      </c>
+      <c r="G515" t="s">
+        <v>689</v>
+      </c>
+      <c r="H515">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B516" t="s">
+        <v>721</v>
+      </c>
+      <c r="C516" t="s">
+        <v>528</v>
+      </c>
+      <c r="D516" t="s">
+        <v>722</v>
+      </c>
+      <c r="E516" t="s">
+        <v>86</v>
+      </c>
+      <c r="F516" t="s">
+        <v>166</v>
+      </c>
+      <c r="G516" t="s">
+        <v>689</v>
+      </c>
+      <c r="H516">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B517" t="s">
+        <v>723</v>
+      </c>
+      <c r="C517" t="s">
+        <v>459</v>
+      </c>
+      <c r="D517" t="s">
+        <v>724</v>
+      </c>
+      <c r="E517" t="s">
+        <v>86</v>
+      </c>
+      <c r="F517" t="s">
+        <v>166</v>
+      </c>
+      <c r="G517" t="s">
+        <v>689</v>
+      </c>
+      <c r="H517">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B518" t="s">
+        <v>725</v>
+      </c>
+      <c r="C518" t="s">
+        <v>726</v>
+      </c>
+      <c r="D518" t="s">
+        <v>727</v>
+      </c>
+      <c r="E518" t="s">
+        <v>86</v>
+      </c>
+      <c r="F518" t="s">
+        <v>166</v>
+      </c>
+      <c r="G518" t="s">
+        <v>689</v>
+      </c>
+      <c r="H518">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B519" t="s">
+        <v>728</v>
+      </c>
+      <c r="C519" t="s">
+        <v>444</v>
+      </c>
+      <c r="D519" t="s">
+        <v>729</v>
+      </c>
+      <c r="E519" t="s">
+        <v>86</v>
+      </c>
+      <c r="F519" t="s">
+        <v>166</v>
+      </c>
+      <c r="G519" t="s">
+        <v>689</v>
+      </c>
+      <c r="H519">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B520" t="s">
+        <v>716</v>
+      </c>
+      <c r="C520" t="s">
+        <v>563</v>
+      </c>
+      <c r="D520" t="s">
+        <v>717</v>
+      </c>
+      <c r="E520" t="s">
+        <v>86</v>
+      </c>
+      <c r="F520" t="s">
+        <v>166</v>
+      </c>
+      <c r="G520" t="s">
+        <v>689</v>
+      </c>
+      <c r="H520">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B521" t="s">
+        <v>730</v>
+      </c>
+      <c r="C521" t="s">
+        <v>731</v>
+      </c>
+      <c r="D521" t="s">
+        <v>732</v>
+      </c>
+      <c r="E521" t="s">
+        <v>86</v>
+      </c>
+      <c r="F521" t="s">
+        <v>166</v>
+      </c>
+      <c r="G521" t="s">
+        <v>689</v>
+      </c>
+      <c r="H521">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B522" t="s">
+        <v>733</v>
+      </c>
+      <c r="C522" t="s">
+        <v>734</v>
+      </c>
+      <c r="D522" t="s">
+        <v>735</v>
+      </c>
+      <c r="E522" t="s">
+        <v>86</v>
+      </c>
+      <c r="F522" t="s">
+        <v>166</v>
+      </c>
+      <c r="G522" t="s">
+        <v>689</v>
+      </c>
+      <c r="H522">
         <v>2</v>
       </c>
     </row>

</xml_diff>